<commit_message>
Added levelTargets to combine chains
</commit_message>
<xml_diff>
--- a/data/neurons.xlsx
+++ b/data/neurons.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="544">
   <si>
     <t>id</t>
   </si>
@@ -781,6 +781,246 @@
     <t>wbkg:lt-cell-cyst</t>
   </si>
   <si>
+    <t>mmset1/11_n1</t>
+  </si>
+  <si>
+    <t>mmset1/11_n14</t>
+  </si>
+  <si>
+    <t>mmset1/11_n16</t>
+  </si>
+  <si>
+    <t>mmset1/11_n18</t>
+  </si>
+  <si>
+    <t>mmset1/11_n20</t>
+  </si>
+  <si>
+    <t>mmset1/12_n1</t>
+  </si>
+  <si>
+    <t>mmset1/12_n8</t>
+  </si>
+  <si>
+    <t>mmset1/12_n10</t>
+  </si>
+  <si>
+    <t>mmset1/12_n12</t>
+  </si>
+  <si>
+    <t>mmset1/12_n14</t>
+  </si>
+  <si>
+    <t>mmset4/1_n1</t>
+  </si>
+  <si>
+    <t>mmset4/1_n5</t>
+  </si>
+  <si>
+    <t>mmset4/1_n7</t>
+  </si>
+  <si>
+    <t>mmset4/2_n1</t>
+  </si>
+  <si>
+    <t>mmset4/2_n6</t>
+  </si>
+  <si>
+    <t>mmset4/3a_n1</t>
+  </si>
+  <si>
+    <t>mmset4/3a_n5</t>
+  </si>
+  <si>
+    <t>mmset4/3b_n1</t>
+  </si>
+  <si>
+    <t>mmset4/3b_n5</t>
+  </si>
+  <si>
+    <t>mmset4/3c_n1</t>
+  </si>
+  <si>
+    <t>mmset4/3c_n5</t>
+  </si>
+  <si>
+    <t>mmset4/7_n1</t>
+  </si>
+  <si>
+    <t>mmset4/7_n6</t>
+  </si>
+  <si>
+    <t>mmset4/7_n8</t>
+  </si>
+  <si>
+    <t>mmset4/7_n10</t>
+  </si>
+  <si>
+    <t>mmset4/7_n12</t>
+  </si>
+  <si>
+    <t>mmset4/7_n14</t>
+  </si>
+  <si>
+    <t>mmset4/7_n16</t>
+  </si>
+  <si>
+    <t>mmset4/7_n18</t>
+  </si>
+  <si>
+    <t>mmset4/7_n20</t>
+  </si>
+  <si>
+    <t>mmset4/7_n22</t>
+  </si>
+  <si>
+    <t>mmset4/7_n24</t>
+  </si>
+  <si>
+    <t>mmset4/7_n26</t>
+  </si>
+  <si>
+    <t>mmset4/8_n1</t>
+  </si>
+  <si>
+    <t>mmset4/8_n6</t>
+  </si>
+  <si>
+    <t>mmset4/8_n8</t>
+  </si>
+  <si>
+    <t>mmset4/8_n10</t>
+  </si>
+  <si>
+    <t>mmset4/8_n12</t>
+  </si>
+  <si>
+    <t>mmset4/11_n1</t>
+  </si>
+  <si>
+    <t>mmset4/11_n5</t>
+  </si>
+  <si>
+    <t>mmset4/11_n7</t>
+  </si>
+  <si>
+    <t>mmset4/11_n9</t>
+  </si>
+  <si>
+    <t>mmset4/12_n1</t>
+  </si>
+  <si>
+    <t>mmset4/12_n5</t>
+  </si>
+  <si>
+    <t>mmset4/12_n7</t>
+  </si>
+  <si>
+    <t>mmset4/12_n9</t>
+  </si>
+  <si>
+    <t>prostate/11_n1</t>
+  </si>
+  <si>
+    <t>prostate/11_n6</t>
+  </si>
+  <si>
+    <t>prostate/11_n8</t>
+  </si>
+  <si>
+    <t>prostate/13_n1</t>
+  </si>
+  <si>
+    <t>prostate/13_n5</t>
+  </si>
+  <si>
+    <t>prostate/15_n1</t>
+  </si>
+  <si>
+    <t>prostate/15_n6</t>
+  </si>
+  <si>
+    <t>prostate/15_n8</t>
+  </si>
+  <si>
+    <t>prostate/15_n10</t>
+  </si>
+  <si>
+    <t>prostate/15_n12</t>
+  </si>
+  <si>
+    <t>prostate/17_n1</t>
+  </si>
+  <si>
+    <t>prostate/17_n5</t>
+  </si>
+  <si>
+    <t>prostate/17_n7</t>
+  </si>
+  <si>
+    <t>prostate/24_n1</t>
+  </si>
+  <si>
+    <t>prostate/24_n5</t>
+  </si>
+  <si>
+    <t>prostate/24_n7</t>
+  </si>
+  <si>
+    <t>prostate/24_n9</t>
+  </si>
+  <si>
+    <t>prostate/26_n1</t>
+  </si>
+  <si>
+    <t>prostate/26_n4</t>
+  </si>
+  <si>
+    <t>prostate/26_n7</t>
+  </si>
+  <si>
+    <t>prostate/26_n9</t>
+  </si>
+  <si>
+    <t>semves/1_n1</t>
+  </si>
+  <si>
+    <t>semves/1_n6</t>
+  </si>
+  <si>
+    <t>semves/3_n1</t>
+  </si>
+  <si>
+    <t>semves/3_n4</t>
+  </si>
+  <si>
+    <t>semves/5_n1</t>
+  </si>
+  <si>
+    <t>semves/5_n4</t>
+  </si>
+  <si>
+    <t>semves/5_n8</t>
+  </si>
+  <si>
+    <t>semves/5_n10</t>
+  </si>
+  <si>
+    <t>semves/5_n12</t>
+  </si>
+  <si>
+    <t>semves/5_n14</t>
+  </si>
+  <si>
+    <t>semves/7_n1</t>
+  </si>
+  <si>
+    <t>semves/7_n5</t>
+  </si>
+  <si>
+    <t>semves/7_n7</t>
+  </si>
+  <si>
     <t>wbkg:lyph-CNS-nucleus-Onuf,wbkg:lyph-PNS-nerve-pudendal,wbkg:lyph-urinary-proximal-sphinctered-urethra</t>
   </si>
   <si>
@@ -1085,6 +1325,246 @@
   </si>
   <si>
     <t>wbkg:lyph-PNS-pelvic-ganglion,wbkg:lyph-PNS-nerve-postganglionic-parasympathetic-fiber-generic,wbkg:lyph-male-genital-excretory-duct-of-seminal-vesicle</t>
+  </si>
+  <si>
+    <t>0:mmset1/11_n2,1:mmset1/11_n3,2:mmset1/11_n4,3:mmset1/11_n5,4:mmset1/11_n6,5:mmset1/11_n7,6:mmset1/11_n8,7:mmset1/11_n9,8:mmset1/11_n4,9:mmset1/11_n5,10:mmset1/11_n6,11:mmset1/11_n7,12:mmset1/11_n8,13:mmset1/11_n9,14:mmset1/11_n6,15:mmset1/11_n5,16:mmset1/11_n6,17:mmset1/11_n7,18:mmset1/11_n8,19:mmset1/11_n9,20:mmset1/11_n8,21:mmset1/11_n5,22:mmset1/11_n6,23:mmset1/11_n7,24:mmset1/11_n8,25:mmset1/11_n9,26:mmset1/11_n7,27:mmset1/11_n5,28:mmset1/11_n6,29:mmset1/11_n7,30:mmset1/11_n8,31:mmset1/11_n9,32:mmset1/11_n10,33:mmset1/11_n4,34:mmset1/11_n4,35:mmset1/11_n6,36:mmset1/11_n8,37:mmset1/11_n7,38:mmset1/11_n11,39:mmset1/11_n4,40:mmset1/11_n4,41:mmset1/11_n6,42:mmset1/11_n8,43:mmset1/11_n7,44:mmset1/11_n12,45:mmset1/11_n4,46:mmset1/11_n4,47:mmset1/11_n6,48:mmset1/11_n8,49:mmset1/11_n7,50:mmset1/11_n13,51:mmset1/11_n4,52:mmset1/11_n4,53:mmset1/11_n6,54:mmset1/11_n8,55:mmset1/11_n7</t>
+  </si>
+  <si>
+    <t>0:mmset1/11_n15,1:mmset1/11_n3,2:mmset1/11_n10,3:mmset1/11_n11,4:mmset1/11_n12,5:mmset1/11_n13</t>
+  </si>
+  <si>
+    <t>0:mmset1/11_n17,1:mmset1/11_n3,2:mmset1/11_n10,3:mmset1/11_n11,4:mmset1/11_n12,5:mmset1/11_n13</t>
+  </si>
+  <si>
+    <t>0:mmset1/11_n19,1:mmset1/11_n3,2:mmset1/11_n10,3:mmset1/11_n11,4:mmset1/11_n12,5:mmset1/11_n13</t>
+  </si>
+  <si>
+    <t>0:mmset1/11_n21,1:mmset1/11_n3,2:mmset1/11_n10,3:mmset1/11_n11,4:mmset1/11_n12,5:mmset1/11_n13</t>
+  </si>
+  <si>
+    <t>0:mmset1/12_n2,1:mmset1/12_n3,2:mmset1/12_n4,3:mmset1/12_n5,4:mmset1/12_n6,5:mmset1/12_n7</t>
+  </si>
+  <si>
+    <t>0:mmset1/12_n9,1:mmset1/12_n3,2:mmset1/12_n4,3:mmset1/12_n5,4:mmset1/12_n6,5:mmset1/12_n7</t>
+  </si>
+  <si>
+    <t>0:mmset1/12_n11,1:mmset1/12_n3,2:mmset1/12_n4,3:mmset1/12_n5,4:mmset1/12_n6,5:mmset1/12_n7</t>
+  </si>
+  <si>
+    <t>0:mmset1/12_n13,1:mmset1/12_n3,2:mmset1/12_n4,3:mmset1/12_n5,4:mmset1/12_n6,5:mmset1/12_n7</t>
+  </si>
+  <si>
+    <t>0:mmset1/12_n15,1:mmset1/12_n3,2:mmset1/12_n16,3:mmset1/12_n4,4:mmset1/12_n16,5:mmset1/12_n5,6:mmset1/12_n16,7:mmset1/12_n6,8:mmset1/12_n16,9:mmset1/12_n7,10:mmset1/12_n16,11:mmset1/12_n17</t>
+  </si>
+  <si>
+    <t>0:mmset4/1_n2,1:mmset4/1_n3,2:mmset4/1_n4</t>
+  </si>
+  <si>
+    <t>0:mmset4/1_n6,1:mmset4/1_n3</t>
+  </si>
+  <si>
+    <t>0:mmset4/1_n8,1:mmset4/1_n3</t>
+  </si>
+  <si>
+    <t>0:mmset4/2_n2,1:mmset4/2_n3,2:mmset4/2_n4,3:mmset4/2_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/2_n7,1:mmset4/2_n3</t>
+  </si>
+  <si>
+    <t>0:mmset4/3a_n2,1:mmset4/3a_n3,2:mmset4/3a_n4</t>
+  </si>
+  <si>
+    <t>0:mmset4/3a_n6,1:mmset4/3a_n3</t>
+  </si>
+  <si>
+    <t>0:mmset4/3b_n2,1:mmset4/3b_n3,2:mmset4/3b_n4</t>
+  </si>
+  <si>
+    <t>0:mmset4/3b_n6,1:mmset4/3b_n3</t>
+  </si>
+  <si>
+    <t>0:mmset4/3c_n2,1:mmset4/3c_n3,2:mmset4/3c_n4</t>
+  </si>
+  <si>
+    <t>0:mmset4/3c_n6,1:mmset4/3c_n3</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n2,1:mmset4/7_n3,2:mmset4/7_n4,3:mmset4/7_n5,4:mmset4/7_n4</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n7,1:mmset4/7_n3,2:mmset4/7_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n9,1:mmset4/7_n3,2:mmset4/7_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n11,1:mmset4/7_n3,2:mmset4/7_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n13,1:mmset4/7_n3,2:mmset4/7_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n15,1:mmset4/7_n3,2:mmset4/7_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n17,1:mmset4/7_n3,2:mmset4/7_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n19,1:mmset4/7_n3,2:mmset4/7_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n21,1:mmset4/7_n3,2:mmset4/7_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n23,1:mmset4/7_n3,2:mmset4/7_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n25,1:mmset4/7_n3,2:mmset4/7_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/7_n27,1:mmset4/7_n3,2:mmset4/7_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/8_n2,1:mmset4/8_n3,2:mmset4/8_n4,3:mmset4/8_n5,4:mmset4/8_n4</t>
+  </si>
+  <si>
+    <t>0:mmset4/8_n7,1:mmset4/8_n3,2:mmset4/8_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/8_n9,1:mmset4/8_n3,2:mmset4/8_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/8_n11,1:mmset4/8_n3,2:mmset4/8_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/8_n13,1:mmset4/8_n3,2:mmset4/8_n5</t>
+  </si>
+  <si>
+    <t>0:mmset4/11_n2,1:mmset4/11_n3,2:mmset4/11_n4</t>
+  </si>
+  <si>
+    <t>0:mmset4/11_n6,1:mmset4/11_n3</t>
+  </si>
+  <si>
+    <t>0:mmset4/11_n8,1:mmset4/11_n3</t>
+  </si>
+  <si>
+    <t>0:mmset4/11_n10,1:mmset4/11_n3</t>
+  </si>
+  <si>
+    <t>0:mmset4/12_n2,1:mmset4/12_n3,2:mmset4/12_n4</t>
+  </si>
+  <si>
+    <t>0:mmset4/12_n6,1:mmset4/12_n3</t>
+  </si>
+  <si>
+    <t>0:mmset4/12_n8,1:mmset4/12_n3</t>
+  </si>
+  <si>
+    <t>0:mmset4/12_n10,1:mmset4/12_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/11_n2,1:prostate/11_n3,2:prostate/11_n4,3:prostate/11_n5</t>
+  </si>
+  <si>
+    <t>0:prostate/11_n7,1:prostate/11_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/11_n9,1:prostate/11_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/13_n2,1:prostate/13_n3,2:prostate/13_n4</t>
+  </si>
+  <si>
+    <t>0:prostate/13_n6,1:prostate/13_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/15_n2,1:prostate/15_n3,2:prostate/15_n4,3:prostate/15_n5</t>
+  </si>
+  <si>
+    <t>0:prostate/15_n7,1:prostate/15_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/15_n9,1:prostate/15_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/15_n11,1:prostate/15_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/15_n13,1:prostate/15_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/17_n2,1:prostate/17_n3,2:prostate/17_n4</t>
+  </si>
+  <si>
+    <t>0:prostate/17_n6,1:prostate/17_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/17_n8,1:prostate/17_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/24_n2,1:prostate/24_n3,2:prostate/24_n4</t>
+  </si>
+  <si>
+    <t>0:prostate/24_n6,1:prostate/24_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/24_n8,1:prostate/24_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/24_n10,1:prostate/24_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/26_n2,1:prostate/26_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/26_n5,1:prostate/26_n3,2:prostate/26_n6</t>
+  </si>
+  <si>
+    <t>0:prostate/26_n8,1:prostate/26_n3</t>
+  </si>
+  <si>
+    <t>0:prostate/26_n10,1:prostate/26_n3</t>
+  </si>
+  <si>
+    <t>0:semves/1_n2,1:semves/1_n3,2:semves/1_n4,3:semves/1_n5</t>
+  </si>
+  <si>
+    <t>0:semves/1_n7,1:semves/1_n3</t>
+  </si>
+  <si>
+    <t>0:semves/3_n2,1:semves/3_n3</t>
+  </si>
+  <si>
+    <t>0:semves/3_n5,1:semves/3_n3,2:semves/3_n6</t>
+  </si>
+  <si>
+    <t>0:semves/5_n2,1:semves/5_n3</t>
+  </si>
+  <si>
+    <t>0:semves/5_n5,1:semves/5_n3,2:semves/5_n6,3:semves/5_n7</t>
+  </si>
+  <si>
+    <t>0:semves/5_n9,1:semves/5_n3</t>
+  </si>
+  <si>
+    <t>0:semves/5_n11,1:semves/5_n3</t>
+  </si>
+  <si>
+    <t>0:semves/5_n13,1:semves/5_n3</t>
+  </si>
+  <si>
+    <t>0:semves/5_n15,1:semves/5_n3</t>
+  </si>
+  <si>
+    <t>0:semves/7_n2,1:semves/7_n3,2:semves/7_n4</t>
+  </si>
+  <si>
+    <t>0:semves/7_n6,1:semves/7_n3</t>
+  </si>
+  <si>
+    <t>0:semves/7_n8,1:semves/7_n3</t>
   </si>
   <si>
     <t>lyphs</t>
@@ -1635,7 +2115,7 @@
         <v>253</v>
       </c>
       <c r="F2" t="s">
-        <v>254</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1649,7 +2129,7 @@
         <v>253</v>
       </c>
       <c r="F3" t="s">
-        <v>255</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1663,7 +2143,7 @@
         <v>253</v>
       </c>
       <c r="F4" t="s">
-        <v>256</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1677,7 +2157,7 @@
         <v>253</v>
       </c>
       <c r="F5" t="s">
-        <v>257</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1691,7 +2171,7 @@
         <v>253</v>
       </c>
       <c r="F6" t="s">
-        <v>258</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1705,7 +2185,7 @@
         <v>253</v>
       </c>
       <c r="F7" t="s">
-        <v>259</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1719,7 +2199,7 @@
         <v>253</v>
       </c>
       <c r="F8" t="s">
-        <v>260</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1732,8 +2212,14 @@
       <c r="C9" t="s">
         <v>253</v>
       </c>
+      <c r="D9" t="s">
+        <v>254</v>
+      </c>
       <c r="F9" t="s">
-        <v>261</v>
+        <v>341</v>
+      </c>
+      <c r="G9" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1746,8 +2232,14 @@
       <c r="C10" t="s">
         <v>253</v>
       </c>
+      <c r="D10" t="s">
+        <v>255</v>
+      </c>
       <c r="F10" t="s">
-        <v>262</v>
+        <v>342</v>
+      </c>
+      <c r="G10" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1760,8 +2252,14 @@
       <c r="C11" t="s">
         <v>253</v>
       </c>
+      <c r="D11" t="s">
+        <v>256</v>
+      </c>
       <c r="F11" t="s">
-        <v>263</v>
+        <v>343</v>
+      </c>
+      <c r="G11" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1774,8 +2272,14 @@
       <c r="C12" t="s">
         <v>253</v>
       </c>
+      <c r="D12" t="s">
+        <v>257</v>
+      </c>
       <c r="F12" t="s">
-        <v>264</v>
+        <v>344</v>
+      </c>
+      <c r="G12" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1788,8 +2292,14 @@
       <c r="C13" t="s">
         <v>253</v>
       </c>
+      <c r="D13" t="s">
+        <v>258</v>
+      </c>
       <c r="F13" t="s">
-        <v>265</v>
+        <v>345</v>
+      </c>
+      <c r="G13" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1802,8 +2312,14 @@
       <c r="C14" t="s">
         <v>253</v>
       </c>
+      <c r="D14" t="s">
+        <v>259</v>
+      </c>
       <c r="F14" t="s">
-        <v>266</v>
+        <v>346</v>
+      </c>
+      <c r="G14" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1816,8 +2332,14 @@
       <c r="C15" t="s">
         <v>253</v>
       </c>
+      <c r="D15" t="s">
+        <v>260</v>
+      </c>
       <c r="F15" t="s">
-        <v>267</v>
+        <v>347</v>
+      </c>
+      <c r="G15" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1830,11 +2352,17 @@
       <c r="C16" t="s">
         <v>253</v>
       </c>
+      <c r="D16" t="s">
+        <v>261</v>
+      </c>
       <c r="F16" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>348</v>
+      </c>
+      <c r="G16" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1844,11 +2372,17 @@
       <c r="C17" t="s">
         <v>253</v>
       </c>
+      <c r="D17" t="s">
+        <v>262</v>
+      </c>
       <c r="F17" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>349</v>
+      </c>
+      <c r="G17" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1858,11 +2392,17 @@
       <c r="C18" t="s">
         <v>253</v>
       </c>
+      <c r="D18" t="s">
+        <v>263</v>
+      </c>
       <c r="F18" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>350</v>
+      </c>
+      <c r="G18" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1873,10 +2413,10 @@
         <v>253</v>
       </c>
       <c r="F19" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1887,10 +2427,10 @@
         <v>253</v>
       </c>
       <c r="F20" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1901,10 +2441,10 @@
         <v>253</v>
       </c>
       <c r="F21" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -1915,10 +2455,10 @@
         <v>253</v>
       </c>
       <c r="F22" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1929,10 +2469,10 @@
         <v>253</v>
       </c>
       <c r="F23" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1943,10 +2483,10 @@
         <v>253</v>
       </c>
       <c r="F24" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -1957,10 +2497,10 @@
         <v>253</v>
       </c>
       <c r="F25" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1971,10 +2511,10 @@
         <v>253</v>
       </c>
       <c r="F26" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1985,10 +2525,10 @@
         <v>253</v>
       </c>
       <c r="F27" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1999,10 +2539,10 @@
         <v>253</v>
       </c>
       <c r="F28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -2013,10 +2553,10 @@
         <v>253</v>
       </c>
       <c r="F29" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -2027,10 +2567,10 @@
         <v>253</v>
       </c>
       <c r="F30" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2040,11 +2580,17 @@
       <c r="C31" t="s">
         <v>253</v>
       </c>
+      <c r="D31" t="s">
+        <v>264</v>
+      </c>
       <c r="F31" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>363</v>
+      </c>
+      <c r="G31" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -2054,11 +2600,17 @@
       <c r="C32" t="s">
         <v>253</v>
       </c>
+      <c r="D32" t="s">
+        <v>265</v>
+      </c>
       <c r="F32" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>364</v>
+      </c>
+      <c r="G32" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -2068,11 +2620,17 @@
       <c r="C33" t="s">
         <v>253</v>
       </c>
+      <c r="D33" t="s">
+        <v>266</v>
+      </c>
       <c r="F33" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>365</v>
+      </c>
+      <c r="G33" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -2082,11 +2640,17 @@
       <c r="C34" t="s">
         <v>253</v>
       </c>
+      <c r="D34" t="s">
+        <v>267</v>
+      </c>
       <c r="F34" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>366</v>
+      </c>
+      <c r="G34" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -2096,11 +2660,17 @@
       <c r="C35" t="s">
         <v>253</v>
       </c>
+      <c r="D35" t="s">
+        <v>268</v>
+      </c>
       <c r="F35" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>367</v>
+      </c>
+      <c r="G35" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -2111,10 +2681,10 @@
         <v>253</v>
       </c>
       <c r="F36" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -2124,11 +2694,17 @@
       <c r="C37" t="s">
         <v>253</v>
       </c>
+      <c r="D37" t="s">
+        <v>269</v>
+      </c>
       <c r="F37" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>369</v>
+      </c>
+      <c r="G37" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -2138,11 +2714,17 @@
       <c r="C38" t="s">
         <v>253</v>
       </c>
+      <c r="D38" t="s">
+        <v>270</v>
+      </c>
       <c r="F38" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>370</v>
+      </c>
+      <c r="G38" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -2152,11 +2734,17 @@
       <c r="C39" t="s">
         <v>253</v>
       </c>
+      <c r="D39" t="s">
+        <v>271</v>
+      </c>
       <c r="F39" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>371</v>
+      </c>
+      <c r="G39" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -2166,11 +2754,17 @@
       <c r="C40" t="s">
         <v>253</v>
       </c>
+      <c r="D40" t="s">
+        <v>272</v>
+      </c>
       <c r="F40" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>370</v>
+      </c>
+      <c r="G40" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -2180,11 +2774,17 @@
       <c r="C41" t="s">
         <v>253</v>
       </c>
+      <c r="D41" t="s">
+        <v>273</v>
+      </c>
       <c r="F41" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>372</v>
+      </c>
+      <c r="G41" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -2194,11 +2794,17 @@
       <c r="C42" t="s">
         <v>253</v>
       </c>
+      <c r="D42" t="s">
+        <v>274</v>
+      </c>
       <c r="F42" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>370</v>
+      </c>
+      <c r="G42" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2209,10 +2815,10 @@
         <v>253</v>
       </c>
       <c r="F43" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -2223,10 +2829,10 @@
         <v>253</v>
       </c>
       <c r="F44" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -2237,10 +2843,10 @@
         <v>253</v>
       </c>
       <c r="F45" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -2251,10 +2857,10 @@
         <v>253</v>
       </c>
       <c r="F46" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -2265,10 +2871,10 @@
         <v>253</v>
       </c>
       <c r="F47" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -2279,10 +2885,10 @@
         <v>253</v>
       </c>
       <c r="F48" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>64</v>
       </c>
@@ -2292,11 +2898,17 @@
       <c r="C49" t="s">
         <v>253</v>
       </c>
+      <c r="D49" t="s">
+        <v>275</v>
+      </c>
       <c r="F49" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>379</v>
+      </c>
+      <c r="G49" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>65</v>
       </c>
@@ -2306,11 +2918,17 @@
       <c r="C50" t="s">
         <v>253</v>
       </c>
+      <c r="D50" t="s">
+        <v>276</v>
+      </c>
       <c r="F50" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>380</v>
+      </c>
+      <c r="G50" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -2320,11 +2938,17 @@
       <c r="C51" t="s">
         <v>253</v>
       </c>
+      <c r="D51" t="s">
+        <v>277</v>
+      </c>
       <c r="F51" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>381</v>
+      </c>
+      <c r="G51" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -2334,11 +2958,17 @@
       <c r="C52" t="s">
         <v>253</v>
       </c>
+      <c r="D52" t="s">
+        <v>278</v>
+      </c>
       <c r="F52" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>382</v>
+      </c>
+      <c r="G52" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -2348,11 +2978,17 @@
       <c r="C53" t="s">
         <v>253</v>
       </c>
+      <c r="D53" t="s">
+        <v>279</v>
+      </c>
       <c r="F53" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>383</v>
+      </c>
+      <c r="G53" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>69</v>
       </c>
@@ -2362,11 +2998,17 @@
       <c r="C54" t="s">
         <v>253</v>
       </c>
+      <c r="D54" t="s">
+        <v>280</v>
+      </c>
       <c r="F54" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>384</v>
+      </c>
+      <c r="G54" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -2376,11 +3018,17 @@
       <c r="C55" t="s">
         <v>253</v>
       </c>
+      <c r="D55" t="s">
+        <v>281</v>
+      </c>
       <c r="F55" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>385</v>
+      </c>
+      <c r="G55" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -2390,11 +3038,17 @@
       <c r="C56" t="s">
         <v>253</v>
       </c>
+      <c r="D56" t="s">
+        <v>282</v>
+      </c>
       <c r="F56" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>386</v>
+      </c>
+      <c r="G56" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -2404,11 +3058,17 @@
       <c r="C57" t="s">
         <v>253</v>
       </c>
+      <c r="D57" t="s">
+        <v>283</v>
+      </c>
       <c r="F57" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>387</v>
+      </c>
+      <c r="G57" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -2418,11 +3078,17 @@
       <c r="C58" t="s">
         <v>253</v>
       </c>
+      <c r="D58" t="s">
+        <v>284</v>
+      </c>
       <c r="F58" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>388</v>
+      </c>
+      <c r="G58" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -2432,11 +3098,17 @@
       <c r="C59" t="s">
         <v>253</v>
       </c>
+      <c r="D59" t="s">
+        <v>285</v>
+      </c>
       <c r="F59" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>389</v>
+      </c>
+      <c r="G59" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -2446,11 +3118,17 @@
       <c r="C60" t="s">
         <v>253</v>
       </c>
+      <c r="D60" t="s">
+        <v>286</v>
+      </c>
       <c r="F60" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+        <v>390</v>
+      </c>
+      <c r="G60" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -2460,11 +3138,17 @@
       <c r="C61" t="s">
         <v>253</v>
       </c>
+      <c r="D61" t="s">
+        <v>287</v>
+      </c>
       <c r="F61" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+        <v>391</v>
+      </c>
+      <c r="G61" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -2474,11 +3158,17 @@
       <c r="C62" t="s">
         <v>253</v>
       </c>
+      <c r="D62" t="s">
+        <v>288</v>
+      </c>
       <c r="F62" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+        <v>381</v>
+      </c>
+      <c r="G62" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -2488,11 +3178,17 @@
       <c r="C63" t="s">
         <v>253</v>
       </c>
+      <c r="D63" t="s">
+        <v>289</v>
+      </c>
       <c r="F63" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+        <v>382</v>
+      </c>
+      <c r="G63" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -2502,11 +3198,17 @@
       <c r="C64" t="s">
         <v>253</v>
       </c>
+      <c r="D64" t="s">
+        <v>290</v>
+      </c>
       <c r="F64" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+        <v>383</v>
+      </c>
+      <c r="G64" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -2516,11 +3218,17 @@
       <c r="C65" t="s">
         <v>253</v>
       </c>
+      <c r="D65" t="s">
+        <v>291</v>
+      </c>
       <c r="F65" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+        <v>384</v>
+      </c>
+      <c r="G65" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -2531,10 +3239,10 @@
         <v>253</v>
       </c>
       <c r="F66" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -2545,10 +3253,10 @@
         <v>253</v>
       </c>
       <c r="F67" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -2558,11 +3266,17 @@
       <c r="C68" t="s">
         <v>253</v>
       </c>
+      <c r="D68" t="s">
+        <v>292</v>
+      </c>
       <c r="F68" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+        <v>394</v>
+      </c>
+      <c r="G68" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -2572,11 +3286,17 @@
       <c r="C69" t="s">
         <v>253</v>
       </c>
+      <c r="D69" t="s">
+        <v>293</v>
+      </c>
       <c r="F69" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+        <v>395</v>
+      </c>
+      <c r="G69" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -2586,11 +3306,17 @@
       <c r="C70" t="s">
         <v>253</v>
       </c>
+      <c r="D70" t="s">
+        <v>294</v>
+      </c>
       <c r="F70" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+        <v>396</v>
+      </c>
+      <c r="G70" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -2600,11 +3326,17 @@
       <c r="C71" t="s">
         <v>253</v>
       </c>
+      <c r="D71" t="s">
+        <v>295</v>
+      </c>
       <c r="F71" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+        <v>397</v>
+      </c>
+      <c r="G71" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -2614,11 +3346,17 @@
       <c r="C72" t="s">
         <v>253</v>
       </c>
+      <c r="D72" t="s">
+        <v>296</v>
+      </c>
       <c r="F72" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+        <v>398</v>
+      </c>
+      <c r="G72" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -2628,11 +3366,17 @@
       <c r="C73" t="s">
         <v>253</v>
       </c>
+      <c r="D73" t="s">
+        <v>297</v>
+      </c>
       <c r="F73" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+        <v>395</v>
+      </c>
+      <c r="G73" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>89</v>
       </c>
@@ -2642,11 +3386,17 @@
       <c r="C74" t="s">
         <v>253</v>
       </c>
+      <c r="D74" t="s">
+        <v>298</v>
+      </c>
       <c r="F74" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+        <v>396</v>
+      </c>
+      <c r="G74" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>90</v>
       </c>
@@ -2656,11 +3406,17 @@
       <c r="C75" t="s">
         <v>253</v>
       </c>
+      <c r="D75" t="s">
+        <v>299</v>
+      </c>
       <c r="F75" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+        <v>397</v>
+      </c>
+      <c r="G75" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>91</v>
       </c>
@@ -2670,11 +3426,17 @@
       <c r="C76" t="s">
         <v>253</v>
       </c>
+      <c r="D76" t="s">
+        <v>300</v>
+      </c>
       <c r="F76" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+        <v>399</v>
+      </c>
+      <c r="G76" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>92</v>
       </c>
@@ -2684,11 +3446,17 @@
       <c r="C77" t="s">
         <v>253</v>
       </c>
+      <c r="D77" t="s">
+        <v>301</v>
+      </c>
       <c r="F77" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+        <v>400</v>
+      </c>
+      <c r="G77" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>93</v>
       </c>
@@ -2698,11 +3466,17 @@
       <c r="C78" t="s">
         <v>253</v>
       </c>
+      <c r="D78" t="s">
+        <v>302</v>
+      </c>
       <c r="F78" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+        <v>401</v>
+      </c>
+      <c r="G78" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>94</v>
       </c>
@@ -2712,11 +3486,17 @@
       <c r="C79" t="s">
         <v>253</v>
       </c>
+      <c r="D79" t="s">
+        <v>301</v>
+      </c>
       <c r="F79" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+        <v>400</v>
+      </c>
+      <c r="G79" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>95</v>
       </c>
@@ -2726,11 +3506,17 @@
       <c r="C80" t="s">
         <v>253</v>
       </c>
+      <c r="D80" t="s">
+        <v>302</v>
+      </c>
       <c r="F80" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+        <v>401</v>
+      </c>
+      <c r="G80" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>96</v>
       </c>
@@ -2741,10 +3527,10 @@
         <v>253</v>
       </c>
       <c r="F81" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>97</v>
       </c>
@@ -2754,11 +3540,17 @@
       <c r="C82" t="s">
         <v>253</v>
       </c>
+      <c r="D82" t="s">
+        <v>303</v>
+      </c>
       <c r="F82" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+        <v>403</v>
+      </c>
+      <c r="G82" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>98</v>
       </c>
@@ -2768,11 +3560,17 @@
       <c r="C83" t="s">
         <v>253</v>
       </c>
+      <c r="D83" t="s">
+        <v>304</v>
+      </c>
       <c r="F83" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+        <v>404</v>
+      </c>
+      <c r="G83" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>99</v>
       </c>
@@ -2783,10 +3581,10 @@
         <v>253</v>
       </c>
       <c r="F84" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>100</v>
       </c>
@@ -2796,11 +3594,17 @@
       <c r="C85" t="s">
         <v>253</v>
       </c>
+      <c r="D85" t="s">
+        <v>305</v>
+      </c>
       <c r="F85" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+        <v>406</v>
+      </c>
+      <c r="G85" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>101</v>
       </c>
@@ -2810,11 +3614,17 @@
       <c r="C86" t="s">
         <v>253</v>
       </c>
+      <c r="D86" t="s">
+        <v>306</v>
+      </c>
       <c r="F86" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+        <v>407</v>
+      </c>
+      <c r="G86" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>102</v>
       </c>
@@ -2824,11 +3634,17 @@
       <c r="C87" t="s">
         <v>253</v>
       </c>
+      <c r="D87" t="s">
+        <v>307</v>
+      </c>
       <c r="F87" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+        <v>408</v>
+      </c>
+      <c r="G87" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>103</v>
       </c>
@@ -2838,11 +3654,17 @@
       <c r="C88" t="s">
         <v>253</v>
       </c>
+      <c r="D88" t="s">
+        <v>308</v>
+      </c>
       <c r="F88" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+        <v>409</v>
+      </c>
+      <c r="G88" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>104</v>
       </c>
@@ -2852,11 +3674,17 @@
       <c r="C89" t="s">
         <v>253</v>
       </c>
+      <c r="D89" t="s">
+        <v>309</v>
+      </c>
       <c r="F89" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+        <v>410</v>
+      </c>
+      <c r="G89" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>105</v>
       </c>
@@ -2867,10 +3695,10 @@
         <v>253</v>
       </c>
       <c r="F90" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>106</v>
       </c>
@@ -2880,11 +3708,17 @@
       <c r="C91" t="s">
         <v>253</v>
       </c>
+      <c r="D91" t="s">
+        <v>310</v>
+      </c>
       <c r="F91" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+        <v>412</v>
+      </c>
+      <c r="G91" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -2894,11 +3728,17 @@
       <c r="C92" t="s">
         <v>253</v>
       </c>
+      <c r="D92" t="s">
+        <v>311</v>
+      </c>
       <c r="F92" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+        <v>413</v>
+      </c>
+      <c r="G92" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -2908,11 +3748,17 @@
       <c r="C93" t="s">
         <v>253</v>
       </c>
+      <c r="D93" t="s">
+        <v>312</v>
+      </c>
       <c r="F93" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+        <v>414</v>
+      </c>
+      <c r="G93" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -2923,10 +3769,10 @@
         <v>253</v>
       </c>
       <c r="F94" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -2936,11 +3782,17 @@
       <c r="C95" t="s">
         <v>253</v>
       </c>
+      <c r="D95" t="s">
+        <v>313</v>
+      </c>
       <c r="F95" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+        <v>416</v>
+      </c>
+      <c r="G95" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>111</v>
       </c>
@@ -2950,11 +3802,17 @@
       <c r="C96" t="s">
         <v>253</v>
       </c>
+      <c r="D96" t="s">
+        <v>314</v>
+      </c>
       <c r="F96" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+        <v>417</v>
+      </c>
+      <c r="G96" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
         <v>112</v>
       </c>
@@ -2964,11 +3822,17 @@
       <c r="C97" t="s">
         <v>253</v>
       </c>
+      <c r="D97" t="s">
+        <v>315</v>
+      </c>
       <c r="F97" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+        <v>418</v>
+      </c>
+      <c r="G97" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" t="s">
         <v>113</v>
       </c>
@@ -2978,11 +3842,17 @@
       <c r="C98" t="s">
         <v>253</v>
       </c>
+      <c r="D98" t="s">
+        <v>316</v>
+      </c>
       <c r="F98" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+        <v>419</v>
+      </c>
+      <c r="G98" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -2993,10 +3863,10 @@
         <v>253</v>
       </c>
       <c r="F99" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" t="s">
         <v>115</v>
       </c>
@@ -3006,11 +3876,17 @@
       <c r="C100" t="s">
         <v>253</v>
       </c>
+      <c r="D100" t="s">
+        <v>317</v>
+      </c>
       <c r="F100" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
+        <v>421</v>
+      </c>
+      <c r="G100" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
         <v>116</v>
       </c>
@@ -3020,11 +3896,17 @@
       <c r="C101" t="s">
         <v>253</v>
       </c>
+      <c r="D101" t="s">
+        <v>318</v>
+      </c>
       <c r="F101" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
+        <v>422</v>
+      </c>
+      <c r="G101" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102" t="s">
         <v>117</v>
       </c>
@@ -3034,11 +3916,17 @@
       <c r="C102" t="s">
         <v>253</v>
       </c>
+      <c r="D102" t="s">
+        <v>319</v>
+      </c>
       <c r="F102" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
+        <v>423</v>
+      </c>
+      <c r="G102" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103" t="s">
         <v>118</v>
       </c>
@@ -3048,11 +3936,17 @@
       <c r="C103" t="s">
         <v>253</v>
       </c>
+      <c r="D103" t="s">
+        <v>320</v>
+      </c>
       <c r="F103" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
+        <v>413</v>
+      </c>
+      <c r="G103" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104" t="s">
         <v>119</v>
       </c>
@@ -3062,11 +3956,17 @@
       <c r="C104" t="s">
         <v>253</v>
       </c>
+      <c r="D104" t="s">
+        <v>321</v>
+      </c>
       <c r="F104" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
+        <v>424</v>
+      </c>
+      <c r="G104" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105" t="s">
         <v>120</v>
       </c>
@@ -3076,11 +3976,17 @@
       <c r="C105" t="s">
         <v>253</v>
       </c>
+      <c r="D105" t="s">
+        <v>322</v>
+      </c>
       <c r="F105" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
+        <v>425</v>
+      </c>
+      <c r="G105" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106" t="s">
         <v>121</v>
       </c>
@@ -3091,10 +3997,10 @@
         <v>253</v>
       </c>
       <c r="F106" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107" t="s">
         <v>122</v>
       </c>
@@ -3105,10 +4011,10 @@
         <v>253</v>
       </c>
       <c r="F107" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108" t="s">
         <v>123</v>
       </c>
@@ -3118,11 +4024,17 @@
       <c r="C108" t="s">
         <v>253</v>
       </c>
+      <c r="D108" t="s">
+        <v>323</v>
+      </c>
       <c r="F108" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
+        <v>421</v>
+      </c>
+      <c r="G108" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109" t="s">
         <v>124</v>
       </c>
@@ -3132,11 +4044,17 @@
       <c r="C109" t="s">
         <v>253</v>
       </c>
+      <c r="D109" t="s">
+        <v>324</v>
+      </c>
       <c r="F109" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
+        <v>428</v>
+      </c>
+      <c r="G109" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110" t="s">
         <v>125</v>
       </c>
@@ -3147,10 +4065,10 @@
         <v>253</v>
       </c>
       <c r="F110" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111" t="s">
         <v>126</v>
       </c>
@@ -3161,10 +4079,10 @@
         <v>253</v>
       </c>
       <c r="F111" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112" t="s">
         <v>127</v>
       </c>
@@ -3174,11 +4092,17 @@
       <c r="C112" t="s">
         <v>253</v>
       </c>
+      <c r="D112" t="s">
+        <v>325</v>
+      </c>
       <c r="F112" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
+        <v>408</v>
+      </c>
+      <c r="G112" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113" t="s">
         <v>128</v>
       </c>
@@ -3188,11 +4112,17 @@
       <c r="C113" t="s">
         <v>253</v>
       </c>
+      <c r="D113" t="s">
+        <v>326</v>
+      </c>
       <c r="F113" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
+        <v>431</v>
+      </c>
+      <c r="G113" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114" t="s">
         <v>129</v>
       </c>
@@ -3202,11 +4132,17 @@
       <c r="C114" t="s">
         <v>253</v>
       </c>
+      <c r="D114" t="s">
+        <v>327</v>
+      </c>
       <c r="F114" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
+        <v>410</v>
+      </c>
+      <c r="G114" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115" t="s">
         <v>130</v>
       </c>
@@ -3216,11 +4152,17 @@
       <c r="C115" t="s">
         <v>253</v>
       </c>
+      <c r="D115" t="s">
+        <v>328</v>
+      </c>
       <c r="F115" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
+        <v>432</v>
+      </c>
+      <c r="G115" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116" t="s">
         <v>131</v>
       </c>
@@ -3230,11 +4172,17 @@
       <c r="C116" t="s">
         <v>253</v>
       </c>
+      <c r="D116" t="s">
+        <v>329</v>
+      </c>
       <c r="F116" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
+        <v>433</v>
+      </c>
+      <c r="G116" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117" t="s">
         <v>132</v>
       </c>
@@ -3244,11 +4192,17 @@
       <c r="C117" t="s">
         <v>253</v>
       </c>
+      <c r="D117" t="s">
+        <v>330</v>
+      </c>
       <c r="F117" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
+        <v>407</v>
+      </c>
+      <c r="G117" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
       <c r="A118" t="s">
         <v>133</v>
       </c>
@@ -3259,10 +4213,10 @@
         <v>253</v>
       </c>
       <c r="F118" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119" t="s">
         <v>134</v>
       </c>
@@ -3272,11 +4226,17 @@
       <c r="C119" t="s">
         <v>253</v>
       </c>
+      <c r="D119" t="s">
+        <v>331</v>
+      </c>
       <c r="F119" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
+        <v>412</v>
+      </c>
+      <c r="G119" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
       <c r="A120" t="s">
         <v>135</v>
       </c>
@@ -3286,11 +4246,17 @@
       <c r="C120" t="s">
         <v>253</v>
       </c>
+      <c r="D120" t="s">
+        <v>332</v>
+      </c>
       <c r="F120" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
+        <v>413</v>
+      </c>
+      <c r="G120" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
       <c r="A121" t="s">
         <v>136</v>
       </c>
@@ -3300,11 +4266,17 @@
       <c r="C121" t="s">
         <v>253</v>
       </c>
+      <c r="D121" t="s">
+        <v>333</v>
+      </c>
       <c r="F121" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
+        <v>414</v>
+      </c>
+      <c r="G121" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
       <c r="A122" t="s">
         <v>137</v>
       </c>
@@ -3315,7 +4287,7 @@
         <v>253</v>
       </c>
       <c r="F122" t="s">
-        <v>355</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -3339,7 +4311,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>356</v>
+        <v>516</v>
       </c>
     </row>
   </sheetData>
@@ -3357,7 +4329,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>357</v>
+        <v>517</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -3365,106 +4337,106 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>358</v>
+        <v>518</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>371</v>
+        <v>531</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>359</v>
+        <v>519</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>372</v>
+        <v>532</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>360</v>
+        <v>520</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>373</v>
+        <v>533</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>361</v>
+        <v>521</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>374</v>
+        <v>534</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>522</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>375</v>
+        <v>535</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>363</v>
+        <v>523</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>376</v>
+        <v>536</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>364</v>
+        <v>524</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>377</v>
+        <v>537</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>365</v>
+        <v>525</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>378</v>
+        <v>538</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>366</v>
+        <v>526</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>379</v>
+        <v>539</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>367</v>
+        <v>527</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>380</v>
+        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>368</v>
+        <v>528</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>381</v>
+        <v>541</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>369</v>
+        <v>529</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>382</v>
+        <v>542</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>370</v>
+        <v>530</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>383</v>
+        <v>543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created a branch for hackaton
</commit_message>
<xml_diff>
--- a/data/neurons.xlsx
+++ b/data/neurons.xlsx
@@ -768,6 +768,33 @@
     <t>mmset1/11_lnk_2</t>
   </si>
   <si>
+    <t>mmset1/11_lnk_40</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_3</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_38</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_4</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_37</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_5</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_6</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_7</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_8</t>
+  </si>
+  <si>
     <t>mmset1/11_lnk_23</t>
   </si>
   <si>
@@ -780,37 +807,31 @@
     <t>mmset1/11_lnk_35</t>
   </si>
   <si>
-    <t>mmset1/11_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_4</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_5</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_6</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_7</t>
+    <t>mmset1/11_lnk_9</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_10</t>
   </si>
   <si>
     <t>mmset1/11_lnk_20</t>
   </si>
   <si>
-    <t>mmset1/11_lnk_8</t>
+    <t>mmset1/11_lnk_11</t>
   </si>
   <si>
     <t>mmset1/11_lnk_39</t>
   </si>
   <si>
-    <t>mmset1/11_lnk_9</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_10</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_11</t>
+    <t>mmset1/11_lnk_12</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_13</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_14</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_15</t>
   </si>
   <si>
     <t>mmset1/11_lnk_21</t>
@@ -825,30 +846,9 @@
     <t>mmset1/11_lnk_33</t>
   </si>
   <si>
-    <t>mmset1/11_lnk_12</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_13</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_38</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_14</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_40</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_15</t>
-  </si>
-  <si>
     <t>mmset1/11_lnk_16</t>
   </si>
   <si>
-    <t>mmset1/11_lnk_37</t>
-  </si>
-  <si>
     <t>mmset1/11_lnk_17</t>
   </si>
   <si>
@@ -864,13 +864,34 @@
     <t>mmset1/12_lnk_1</t>
   </si>
   <si>
+    <t>mmset1/12_lnk_2</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_18</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_3</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_4</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_5</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_12</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_6</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_7</t>
+  </si>
+  <si>
     <t>mmset1/12_lnk_14</t>
   </si>
   <si>
-    <t>mmset1/12_lnk_2</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_3</t>
+    <t>mmset1/12_lnk_8</t>
   </si>
   <si>
     <t>mmset1/12_lnk_15</t>
@@ -879,36 +900,15 @@
     <t>mmset1/12_lnk_17</t>
   </si>
   <si>
-    <t>mmset1/12_lnk_4</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_5</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_6</t>
+    <t>mmset1/12_lnk_9</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_10</t>
   </si>
   <si>
     <t>mmset1/12_lnk_16</t>
   </si>
   <si>
-    <t>mmset1/12_lnk_7</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_8</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_18</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_9</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_10</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_12</t>
-  </si>
-  <si>
     <t>mmset1/12_lnk_11</t>
   </si>
   <si>
@@ -993,6 +993,9 @@
     <t>mmset4/7_lnk_4</t>
   </si>
   <si>
+    <t>mmset4/7_lnk_15</t>
+  </si>
+  <si>
     <t>mmset4/7_lnk_5</t>
   </si>
   <si>
@@ -1014,9 +1017,6 @@
     <t>mmset4/7_lnk_11</t>
   </si>
   <si>
-    <t>mmset4/7_lnk_15</t>
-  </si>
-  <si>
     <t>mmset4/7_lnk_12</t>
   </si>
   <si>
@@ -1038,12 +1038,12 @@
     <t>mmset4/8_lnk_3</t>
   </si>
   <si>
+    <t>mmset4/8_lnk_8</t>
+  </si>
+  <si>
     <t>mmset4/8_lnk_4</t>
   </si>
   <si>
-    <t>mmset4/8_lnk_8</t>
-  </si>
-  <si>
     <t>mmset4/8_lnk_5</t>
   </si>
   <si>
@@ -1269,64 +1269,73 @@
     <t>semves/7_lnk_4</t>
   </si>
   <si>
+    <t>Neural segment for ILX:0786141</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0786722</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793211</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793209</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793208</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793698</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0786228</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793617</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793618</t>
+  </si>
+  <si>
+    <t>Neural segment for UBERON:0002441</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793335</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793210</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793699</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793212</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793700</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793336</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793701</t>
+  </si>
+  <si>
     <t>Neural segment for ILX:0786272</t>
   </si>
   <si>
     <t>Neural segment for ILX:0793697</t>
   </si>
   <si>
-    <t>Neural segment for ILX:0793618</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793699</t>
-  </si>
-  <si>
     <t>Neural segment for ILX:0793619</t>
   </si>
   <si>
-    <t>Neural segment for ILX:0793700</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0786141</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793335</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793210</t>
-  </si>
-  <si>
-    <t>Neural segment for UBERON:0002441</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793212</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793336</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793698</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793209</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793211</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0786228</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793208</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0786722</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793617</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793701</t>
+    <t>Neural segment for ILX:0738444</t>
+  </si>
+  <si>
+    <t>Neural segment for UBERON:0001780</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0739304</t>
   </si>
   <si>
     <t>Neural segment for ILX:0784439</t>
@@ -1335,39 +1344,30 @@
     <t>Neural segment for ILX:0790497</t>
   </si>
   <si>
+    <t>Neural segment for ILX:0788945</t>
+  </si>
+  <si>
     <t>Neural segment for ILX:0739303</t>
   </si>
   <si>
-    <t>Neural segment for ILX:0788945</t>
-  </si>
-  <si>
-    <t>Neural segment for UBERON:0001780</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0739304</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0738444</t>
-  </si>
-  <si>
     <t>Neural segment for ILX:0793802</t>
   </si>
   <si>
+    <t>Neural segment for ILX:0793801</t>
+  </si>
+  <si>
     <t>Neural segment for UBERON:0018675</t>
   </si>
   <si>
     <t>Neural segment for ILX:0793800</t>
   </si>
   <si>
-    <t>Neural segment for ILX:0793801</t>
+    <t>Neural segment for ILX:0793804</t>
   </si>
   <si>
     <t>Neural segment for ILX:0793834</t>
   </si>
   <si>
-    <t>Neural segment for ILX:0793804</t>
-  </si>
-  <si>
     <t>Neural segment for ILX:0793805</t>
   </si>
   <si>
@@ -1377,51 +1377,51 @@
     <t>Neural segment for UBERON:0002366</t>
   </si>
   <si>
+    <t>Neural segment for ILX:0793813</t>
+  </si>
+  <si>
+    <t>Neural segment for UBERON:0018681</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793818</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793811</t>
+  </si>
+  <si>
+    <t>Neural segment for UBERON:0018680</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793814</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793817</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793812</t>
+  </si>
+  <si>
     <t>Neural segment for ILX:0793819</t>
   </si>
   <si>
-    <t>Neural segment for UBERON:0018681</t>
+    <t>Neural segment for ILX:0793816</t>
   </si>
   <si>
     <t>Neural segment for ILX:0793815</t>
   </si>
   <si>
-    <t>Neural segment for ILX:0793814</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793813</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793816</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793818</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793817</t>
-  </si>
-  <si>
-    <t>Neural segment for UBERON:0018680</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793811</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793812</t>
-  </si>
-  <si>
     <t>Neural segment for UBERON:0001236</t>
   </si>
   <si>
+    <t>Neural segment for ILX:0793882</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793883</t>
+  </si>
+  <si>
     <t>Neural segment for UBERON:0035770</t>
   </si>
   <si>
-    <t>Neural segment for ILX:0793882</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793883</t>
-  </si>
-  <si>
     <t>Neural segment for ILX:0793877</t>
   </si>
   <si>
@@ -1431,106 +1431,121 @@
     <t>Neural segment for UBERON:0002013</t>
   </si>
   <si>
+    <t>Neural segment for ILX:0793881</t>
+  </si>
+  <si>
     <t>Neural segment for ILX:0793879</t>
   </si>
   <si>
     <t>Neural segment for ILX:0793880</t>
   </si>
   <si>
-    <t>Neural segment for ILX:0793881</t>
+    <t>Neural segment for UBERON:0006447</t>
+  </si>
+  <si>
+    <t>Neural segment for UBERON:0006451</t>
   </si>
   <si>
     <t>Neural segment for UBERON:0006450</t>
   </si>
   <si>
-    <t>Neural segment for UBERON:0006451</t>
-  </si>
-  <si>
     <t>Neural segment for UBERON:0006449</t>
   </si>
   <si>
-    <t>Neural segment for UBERON:0006447</t>
-  </si>
-  <si>
     <t>Neural segment for UBERON:0018683</t>
   </si>
   <si>
+    <t>Neural segment for ILX:0793358</t>
+  </si>
+  <si>
+    <t>Neural segment for UBERON:0006462</t>
+  </si>
+  <si>
     <t>Neural segment for UBERON:0006461</t>
   </si>
   <si>
-    <t>Neural segment for ILX:0793358</t>
-  </si>
-  <si>
     <t>Neural segment for UBERON:0006460</t>
   </si>
   <si>
-    <t>Neural segment for UBERON:0006462</t>
+    <t>Neural segment for UBERON:0006468</t>
+  </si>
+  <si>
+    <t>Neural segment for ILX:0793357</t>
+  </si>
+  <si>
+    <t>Neural segment for UBERON:0006467</t>
+  </si>
+  <si>
+    <t>Neural segment for UBERON:0006448</t>
   </si>
   <si>
     <t>Neural segment for UBERON:0006466</t>
   </si>
   <si>
-    <t>Neural segment for UBERON:0006448</t>
-  </si>
-  <si>
-    <t>Neural segment for UBERON:0006467</t>
-  </si>
-  <si>
-    <t>Neural segment for UBERON:0006468</t>
-  </si>
-  <si>
-    <t>Neural segment for ILX:0793357</t>
-  </si>
-  <si>
     <t>Neural segment for UBERON:0006463</t>
   </si>
   <si>
+    <t>mmset1/11_n4</t>
+  </si>
+  <si>
+    <t>mmset1/11_n7</t>
+  </si>
+  <si>
+    <t>mmset1/11_n15</t>
+  </si>
+  <si>
+    <t>mmset1/11_n9</t>
+  </si>
+  <si>
+    <t>mmset1/11_n2</t>
+  </si>
+  <si>
+    <t>mmset1/11_n22</t>
+  </si>
+  <si>
+    <t>mmset1/11_n5</t>
+  </si>
+  <si>
+    <t>mmset1/11_n8</t>
+  </si>
+  <si>
+    <t>mmset1/11_n3</t>
+  </si>
+  <si>
+    <t>mmset1/11_n12</t>
+  </si>
+  <si>
+    <t>mmset1/11_n23</t>
+  </si>
+  <si>
+    <t>mmset1/11_n18</t>
+  </si>
+  <si>
+    <t>mmset1/11_n24</t>
+  </si>
+  <si>
+    <t>mmset1/11_n25</t>
+  </si>
+  <si>
     <t>mmset1/11_n6</t>
   </si>
   <si>
     <t>mmset1/11_n1</t>
   </si>
   <si>
-    <t>mmset1/11_n9</t>
-  </si>
-  <si>
-    <t>mmset1/11_n23</t>
-  </si>
-  <si>
-    <t>mmset1/11_n24</t>
-  </si>
-  <si>
-    <t>mmset1/11_n4</t>
-  </si>
-  <si>
-    <t>mmset1/11_n3</t>
-  </si>
-  <si>
-    <t>mmset1/11_n12</t>
-  </si>
-  <si>
-    <t>mmset1/11_n8</t>
-  </si>
-  <si>
-    <t>mmset1/11_n18</t>
-  </si>
-  <si>
-    <t>mmset1/11_n22</t>
-  </si>
-  <si>
-    <t>mmset1/11_n15</t>
-  </si>
-  <si>
-    <t>mmset1/11_n5</t>
-  </si>
-  <si>
-    <t>mmset1/11_n2</t>
-  </si>
-  <si>
-    <t>mmset1/11_n7</t>
-  </si>
-  <si>
-    <t>mmset1/11_n25</t>
+    <t>mmset1/12_n1</t>
+  </si>
+  <si>
+    <t>mmset1/12_n6</t>
+  </si>
+  <si>
+    <t>mmset1/12_n10</t>
+  </si>
+  <si>
+    <t>mmset1/12_n11</t>
+  </si>
+  <si>
+    <t>mmset1/12_n3</t>
   </si>
   <si>
     <t>mmset1/12_n9</t>
@@ -1539,72 +1554,60 @@
     <t>mmset1/12_n4</t>
   </si>
   <si>
-    <t>mmset1/12_n10</t>
-  </si>
-  <si>
-    <t>mmset1/12_n3</t>
-  </si>
-  <si>
-    <t>mmset1/12_n1</t>
+    <t>mmset1/12_n8</t>
+  </si>
+  <si>
+    <t>mmset1/12_n5</t>
   </si>
   <si>
     <t>mmset1/12_n2</t>
   </si>
   <si>
-    <t>mmset1/12_n5</t>
-  </si>
-  <si>
-    <t>mmset1/12_n11</t>
-  </si>
-  <si>
-    <t>mmset1/12_n6</t>
-  </si>
-  <si>
-    <t>mmset1/12_n8</t>
-  </si>
-  <si>
     <t>mmset4/1_n3</t>
   </si>
   <si>
     <t>mmset4/1_n6</t>
   </si>
   <si>
+    <t>mmset4/1_n5</t>
+  </si>
+  <si>
     <t>mmset4/1_n2</t>
   </si>
   <si>
     <t>mmset4/1_n1</t>
   </si>
   <si>
-    <t>mmset4/1_n5</t>
+    <t>mmset4/2_n1</t>
+  </si>
+  <si>
+    <t>mmset4/2_n3</t>
+  </si>
+  <si>
+    <t>mmset4/2_n2</t>
   </si>
   <si>
     <t>mmset4/2_n4</t>
   </si>
   <si>
-    <t>mmset4/2_n1</t>
-  </si>
-  <si>
     <t>mmset4/2_n6</t>
   </si>
   <si>
-    <t>mmset4/2_n2</t>
-  </si>
-  <si>
-    <t>mmset4/2_n3</t>
+    <t>mmset4/3a_n3</t>
   </si>
   <si>
     <t>mmset4/3a_n1</t>
   </si>
   <si>
-    <t>mmset4/3a_n3</t>
-  </si>
-  <si>
     <t>mmset4/3a_n2</t>
   </si>
   <si>
     <t>mmset4/3a_n5</t>
   </si>
   <si>
+    <t>mmset4/3b_n3</t>
+  </si>
+  <si>
     <t>mmset4/3b_n1</t>
   </si>
   <si>
@@ -1614,235 +1617,241 @@
     <t>mmset4/3b_n5</t>
   </si>
   <si>
-    <t>mmset4/3b_n3</t>
-  </si>
-  <si>
     <t>mmset4/3c_n1</t>
   </si>
   <si>
+    <t>mmset4/3c_n3</t>
+  </si>
+  <si>
     <t>mmset4/3c_n2</t>
   </si>
   <si>
-    <t>mmset4/3c_n3</t>
-  </si>
-  <si>
     <t>mmset4/3c_n5</t>
   </si>
   <si>
+    <t>mmset4/7_n9</t>
+  </si>
+  <si>
+    <t>mmset4/7_n4</t>
+  </si>
+  <si>
+    <t>mmset4/7_n14</t>
+  </si>
+  <si>
+    <t>mmset4/7_n7</t>
+  </si>
+  <si>
+    <t>mmset4/7_n2</t>
+  </si>
+  <si>
+    <t>mmset4/7_n10</t>
+  </si>
+  <si>
+    <t>mmset4/7_n1</t>
+  </si>
+  <si>
+    <t>mmset4/7_n6</t>
+  </si>
+  <si>
+    <t>mmset4/7_n13</t>
+  </si>
+  <si>
+    <t>mmset4/7_n8</t>
+  </si>
+  <si>
+    <t>mmset4/7_n3</t>
+  </si>
+  <si>
     <t>mmset4/7_n15</t>
   </si>
   <si>
+    <t>mmset4/7_n12</t>
+  </si>
+  <si>
+    <t>mmset4/7_n11</t>
+  </si>
+  <si>
     <t>mmset4/7_n5</t>
   </si>
   <si>
-    <t>mmset4/7_n1</t>
-  </si>
-  <si>
-    <t>mmset4/7_n4</t>
-  </si>
-  <si>
-    <t>mmset4/7_n11</t>
-  </si>
-  <si>
-    <t>mmset4/7_n10</t>
-  </si>
-  <si>
-    <t>mmset4/7_n3</t>
-  </si>
-  <si>
-    <t>mmset4/7_n9</t>
-  </si>
-  <si>
-    <t>mmset4/7_n12</t>
-  </si>
-  <si>
-    <t>mmset4/7_n14</t>
-  </si>
-  <si>
-    <t>mmset4/7_n13</t>
-  </si>
-  <si>
-    <t>mmset4/7_n2</t>
-  </si>
-  <si>
-    <t>mmset4/7_n7</t>
-  </si>
-  <si>
-    <t>mmset4/7_n6</t>
-  </si>
-  <si>
-    <t>mmset4/7_n8</t>
+    <t>mmset4/8_n8</t>
+  </si>
+  <si>
+    <t>mmset4/8_n4</t>
+  </si>
+  <si>
+    <t>mmset4/8_n6</t>
+  </si>
+  <si>
+    <t>mmset4/8_n2</t>
+  </si>
+  <si>
+    <t>mmset4/8_n5</t>
+  </si>
+  <si>
+    <t>mmset4/8_n7</t>
+  </si>
+  <si>
+    <t>mmset4/8_n3</t>
   </si>
   <si>
     <t>mmset4/8_n1</t>
   </si>
   <si>
-    <t>mmset4/8_n4</t>
-  </si>
-  <si>
-    <t>mmset4/8_n3</t>
-  </si>
-  <si>
-    <t>mmset4/8_n8</t>
-  </si>
-  <si>
-    <t>mmset4/8_n2</t>
-  </si>
-  <si>
-    <t>mmset4/8_n6</t>
-  </si>
-  <si>
-    <t>mmset4/8_n5</t>
-  </si>
-  <si>
-    <t>mmset4/8_n7</t>
+    <t>mmset4/11_n6</t>
+  </si>
+  <si>
+    <t>mmset4/11_n2</t>
+  </si>
+  <si>
+    <t>mmset4/11_n5</t>
+  </si>
+  <si>
+    <t>mmset4/11_n7</t>
+  </si>
+  <si>
+    <t>mmset4/11_n3</t>
   </si>
   <si>
     <t>mmset4/11_n1</t>
   </si>
   <si>
-    <t>mmset4/11_n3</t>
-  </si>
-  <si>
-    <t>mmset4/11_n2</t>
-  </si>
-  <si>
-    <t>mmset4/11_n6</t>
-  </si>
-  <si>
-    <t>mmset4/11_n5</t>
-  </si>
-  <si>
-    <t>mmset4/11_n7</t>
+    <t>mmset4/12_n6</t>
+  </si>
+  <si>
+    <t>mmset4/12_n2</t>
+  </si>
+  <si>
+    <t>mmset4/12_n3</t>
+  </si>
+  <si>
+    <t>mmset4/12_n5</t>
+  </si>
+  <si>
+    <t>mmset4/12_n7</t>
   </si>
   <si>
     <t>mmset4/12_n1</t>
   </si>
   <si>
-    <t>mmset4/12_n7</t>
-  </si>
-  <si>
-    <t>mmset4/12_n2</t>
-  </si>
-  <si>
-    <t>mmset4/12_n6</t>
-  </si>
-  <si>
-    <t>mmset4/12_n5</t>
-  </si>
-  <si>
-    <t>mmset4/12_n3</t>
+    <t>prostate/11_n6</t>
+  </si>
+  <si>
+    <t>prostate/11_n8</t>
+  </si>
+  <si>
+    <t>prostate/11_n1</t>
+  </si>
+  <si>
+    <t>prostate/11_n4</t>
+  </si>
+  <si>
+    <t>prostate/11_n3</t>
+  </si>
+  <si>
+    <t>prostate/11_n9</t>
+  </si>
+  <si>
+    <t>prostate/11_n7</t>
   </si>
   <si>
     <t>prostate/11_n2</t>
   </si>
   <si>
-    <t>prostate/11_n7</t>
-  </si>
-  <si>
-    <t>prostate/11_n8</t>
-  </si>
-  <si>
-    <t>prostate/11_n9</t>
-  </si>
-  <si>
-    <t>prostate/11_n3</t>
-  </si>
-  <si>
-    <t>prostate/11_n6</t>
-  </si>
-  <si>
-    <t>prostate/11_n4</t>
-  </si>
-  <si>
-    <t>prostate/11_n1</t>
+    <t>prostate/13_n2</t>
+  </si>
+  <si>
+    <t>prostate/13_n1</t>
   </si>
   <si>
     <t>prostate/13_n3</t>
   </si>
   <si>
-    <t>prostate/13_n1</t>
-  </si>
-  <si>
-    <t>prostate/13_n2</t>
-  </si>
-  <si>
     <t>prostate/13_n5</t>
   </si>
   <si>
+    <t>prostate/15_n8</t>
+  </si>
+  <si>
+    <t>prostate/15_n7</t>
+  </si>
+  <si>
+    <t>prostate/15_n4</t>
+  </si>
+  <si>
+    <t>prostate/15_n3</t>
+  </si>
+  <si>
     <t>prostate/15_n9</t>
   </si>
   <si>
+    <t>prostate/15_n6</t>
+  </si>
+  <si>
     <t>prostate/15_n2</t>
   </si>
   <si>
-    <t>prostate/15_n4</t>
-  </si>
-  <si>
     <t>prostate/15_n1</t>
   </si>
   <si>
-    <t>prostate/15_n3</t>
-  </si>
-  <si>
-    <t>prostate/15_n6</t>
-  </si>
-  <si>
-    <t>prostate/15_n8</t>
-  </si>
-  <si>
-    <t>prostate/15_n7</t>
+    <t>prostate/17_n6</t>
+  </si>
+  <si>
+    <t>prostate/17_n3</t>
+  </si>
+  <si>
+    <t>prostate/17_n2</t>
   </si>
   <si>
     <t>prostate/17_n1</t>
   </si>
   <si>
-    <t>prostate/17_n3</t>
-  </si>
-  <si>
     <t>prostate/17_n5</t>
   </si>
   <si>
-    <t>prostate/17_n2</t>
-  </si>
-  <si>
-    <t>prostate/17_n6</t>
+    <t>prostate/24_n1</t>
+  </si>
+  <si>
+    <t>prostate/24_n7</t>
   </si>
   <si>
     <t>prostate/24_n6</t>
   </si>
   <si>
-    <t>prostate/24_n7</t>
-  </si>
-  <si>
     <t>prostate/24_n3</t>
   </si>
   <si>
     <t>prostate/24_n5</t>
   </si>
   <si>
-    <t>prostate/24_n1</t>
-  </si>
-  <si>
     <t>prostate/24_n2</t>
   </si>
   <si>
+    <t>prostate/26_n1</t>
+  </si>
+  <si>
+    <t>prostate/26_n7</t>
+  </si>
+  <si>
+    <t>prostate/26_n2</t>
+  </si>
+  <si>
+    <t>prostate/26_n3</t>
+  </si>
+  <si>
     <t>prostate/26_n6</t>
   </si>
   <si>
-    <t>prostate/26_n3</t>
-  </si>
-  <si>
-    <t>prostate/26_n1</t>
-  </si>
-  <si>
-    <t>prostate/26_n2</t>
-  </si>
-  <si>
     <t>prostate/26_n4</t>
   </si>
   <si>
-    <t>prostate/26_n7</t>
+    <t>semves/1_n1</t>
+  </si>
+  <si>
+    <t>semves/1_n4</t>
+  </si>
+  <si>
+    <t>semves/1_n3</t>
   </si>
   <si>
     <t>semves/1_n6</t>
@@ -1851,69 +1860,60 @@
     <t>semves/1_n2</t>
   </si>
   <si>
-    <t>semves/1_n3</t>
-  </si>
-  <si>
-    <t>semves/1_n1</t>
-  </si>
-  <si>
-    <t>semves/1_n4</t>
+    <t>semves/3_n2</t>
+  </si>
+  <si>
+    <t>semves/3_n1</t>
+  </si>
+  <si>
+    <t>semves/3_n3</t>
   </si>
   <si>
     <t>semves/3_n4</t>
   </si>
   <si>
-    <t>semves/3_n2</t>
-  </si>
-  <si>
-    <t>semves/3_n3</t>
-  </si>
-  <si>
-    <t>semves/3_n1</t>
+    <t>semves/5_n10</t>
+  </si>
+  <si>
+    <t>semves/5_n1</t>
+  </si>
+  <si>
+    <t>semves/5_n5</t>
+  </si>
+  <si>
+    <t>semves/5_n3</t>
+  </si>
+  <si>
+    <t>semves/5_n9</t>
+  </si>
+  <si>
+    <t>semves/5_n4</t>
   </si>
   <si>
     <t>semves/5_n7</t>
   </si>
   <si>
+    <t>semves/5_n2</t>
+  </si>
+  <si>
     <t>semves/5_n8</t>
   </si>
   <si>
-    <t>semves/5_n4</t>
-  </si>
-  <si>
-    <t>semves/5_n2</t>
-  </si>
-  <si>
-    <t>semves/5_n5</t>
-  </si>
-  <si>
-    <t>semves/5_n9</t>
-  </si>
-  <si>
-    <t>semves/5_n3</t>
-  </si>
-  <si>
-    <t>semves/5_n10</t>
-  </si>
-  <si>
-    <t>semves/5_n1</t>
+    <t>semves/7_n5</t>
+  </si>
+  <si>
+    <t>semves/7_n6</t>
   </si>
   <si>
     <t>semves/7_n3</t>
   </si>
   <si>
+    <t>semves/7_n2</t>
+  </si>
+  <si>
     <t>semves/7_n1</t>
   </si>
   <si>
-    <t>semves/7_n2</t>
-  </si>
-  <si>
-    <t>semves/7_n6</t>
-  </si>
-  <si>
-    <t>semves/7_n5</t>
-  </si>
-  <si>
     <t>mmset1/11_n11</t>
   </si>
   <si>
@@ -1938,15 +1938,15 @@
     <t>mmset1/11_n19</t>
   </si>
   <si>
+    <t>mmset1/12_n13</t>
+  </si>
+  <si>
     <t>mmset1/12_n7</t>
   </si>
   <si>
     <t>mmset1/12_n12</t>
   </si>
   <si>
-    <t>mmset1/12_n13</t>
-  </si>
-  <si>
     <t>mmset4/1_n4</t>
   </si>
   <si>
@@ -3138,250 +3138,250 @@
     <t>semves/8_lyph_0,semves/8_lyph_1,semves/8_lyph_2</t>
   </si>
   <si>
-    <t>mmset1/11_lnk_1,mmset1/11_lnk_16,mmset1/11_lnk_7,mmset1/11_lnk_6,mmset1/11_lnk_15,mmset1/11_lnk_0,mmset1/11_lnk_17,mmset1/11_lnk_9,mmset1/11_lnk_11,mmset1/11_lnk_6,mmset1/11_lnk_15,mmset1/11_lnk_0,mmset1/11_lnk_17,mmset1/11_lnk_9,mmset1/11_lnk_18,mmset1/11_lnk_6,mmset1/11_lnk_15,mmset1/11_lnk_0,mmset1/11_lnk_17,mmset1/11_lnk_9,mmset1/11_lnk_2,mmset1/11_lnk_6,mmset1/11_lnk_15,mmset1/11_lnk_0,mmset1/11_lnk_17,mmset1/11_lnk_9,mmset1/11_lnk_4,mmset1/11_lnk_6,mmset1/11_lnk_15,mmset1/11_lnk_0,mmset1/11_lnk_17,mmset1/11_lnk_9,mmset1/11_lnk_13,mmset1/11_lnk_20,mmset1/11_lnk_21,mmset1/11_lnk_22,mmset1/11_lnk_23,mmset1/11_lnk_24,mmset1/11_lnk_8,mmset1/11_lnk_20,mmset1/11_lnk_25,mmset1/11_lnk_26,mmset1/11_lnk_27,mmset1/11_lnk_28,mmset1/11_lnk_14,mmset1/11_lnk_20,mmset1/11_lnk_29,mmset1/11_lnk_30,mmset1/11_lnk_31,mmset1/11_lnk_32,mmset1/11_lnk_10,mmset1/11_lnk_20,mmset1/11_lnk_33,mmset1/11_lnk_34,mmset1/11_lnk_35,mmset1/11_lnk_36</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_12,mmset1/11_lnk_37,mmset1/11_lnk_38,mmset1/11_lnk_39,mmset1/11_lnk_40,mmset1/11_lnk_10</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_3,mmset1/11_lnk_37,mmset1/11_lnk_38,mmset1/11_lnk_39,mmset1/11_lnk_40,mmset1/11_lnk_10</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_5,mmset1/11_lnk_37,mmset1/11_lnk_38,mmset1/11_lnk_39,mmset1/11_lnk_40,mmset1/11_lnk_10</t>
-  </si>
-  <si>
-    <t>mmset1/11_lnk_19,mmset1/11_lnk_37,mmset1/11_lnk_38,mmset1/11_lnk_39,mmset1/11_lnk_40,mmset1/11_lnk_10</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_4,mmset1/12_lnk_5,mmset1/12_lnk_10,mmset1/12_lnk_1,mmset1/12_lnk_6,mmset1/12_lnk_8</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_9,mmset1/12_lnk_5,mmset1/12_lnk_10,mmset1/12_lnk_1,mmset1/12_lnk_6,mmset1/12_lnk_8</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_0,mmset1/12_lnk_5,mmset1/12_lnk_10,mmset1/12_lnk_1,mmset1/12_lnk_6,mmset1/12_lnk_8</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_2,mmset1/12_lnk_5,mmset1/12_lnk_10,mmset1/12_lnk_1,mmset1/12_lnk_6,mmset1/12_lnk_8</t>
-  </si>
-  <si>
-    <t>mmset1/12_lnk_7,mmset1/12_lnk_5,mmset1/12_lnk_3,mmset1/12_lnk_12,mmset1/12_lnk_13,mmset1/12_lnk_14,mmset1/12_lnk_15,mmset1/12_lnk_16,mmset1/12_lnk_17,mmset1/12_lnk_18,mmset1/12_lnk_17,mmset1/12_lnk_11</t>
-  </si>
-  <si>
-    <t>mmset4/1_lnk_3,mmset4/1_lnk_2,mmset4/1_lnk_0</t>
-  </si>
-  <si>
-    <t>mmset4/1_lnk_4,mmset4/1_lnk_2</t>
-  </si>
-  <si>
-    <t>mmset4/1_lnk_1,mmset4/1_lnk_2</t>
-  </si>
-  <si>
-    <t>mmset4/2_lnk_1,mmset4/2_lnk_3,mmset4/2_lnk_4,mmset4/2_lnk_0</t>
-  </si>
-  <si>
-    <t>mmset4/2_lnk_2,mmset4/2_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/3a_lnk_0,mmset4/3a_lnk_2,mmset4/3a_lnk_1</t>
+    <t>mmset1/11_lnk_18,mmset1/11_lnk_4,mmset1/11_lnk_10,mmset1/11_lnk_0,mmset1/11_lnk_6,mmset1/11_lnk_17,mmset1/11_lnk_1,mmset1/11_lnk_9,mmset1/11_lnk_15,mmset1/11_lnk_0,mmset1/11_lnk_6,mmset1/11_lnk_17,mmset1/11_lnk_1,mmset1/11_lnk_9,mmset1/11_lnk_7,mmset1/11_lnk_0,mmset1/11_lnk_6,mmset1/11_lnk_17,mmset1/11_lnk_1,mmset1/11_lnk_9,mmset1/11_lnk_8,mmset1/11_lnk_0,mmset1/11_lnk_6,mmset1/11_lnk_17,mmset1/11_lnk_1,mmset1/11_lnk_9,mmset1/11_lnk_19,mmset1/11_lnk_0,mmset1/11_lnk_6,mmset1/11_lnk_17,mmset1/11_lnk_1,mmset1/11_lnk_9,mmset1/11_lnk_3,mmset1/11_lnk_20,mmset1/11_lnk_21,mmset1/11_lnk_22,mmset1/11_lnk_23,mmset1/11_lnk_24,mmset1/11_lnk_11,mmset1/11_lnk_20,mmset1/11_lnk_25,mmset1/11_lnk_26,mmset1/11_lnk_27,mmset1/11_lnk_28,mmset1/11_lnk_2,mmset1/11_lnk_20,mmset1/11_lnk_29,mmset1/11_lnk_30,mmset1/11_lnk_31,mmset1/11_lnk_32,mmset1/11_lnk_13,mmset1/11_lnk_20,mmset1/11_lnk_33,mmset1/11_lnk_34,mmset1/11_lnk_35,mmset1/11_lnk_36</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_5,mmset1/11_lnk_37,mmset1/11_lnk_38,mmset1/11_lnk_39,mmset1/11_lnk_40,mmset1/11_lnk_13</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_12,mmset1/11_lnk_37,mmset1/11_lnk_38,mmset1/11_lnk_39,mmset1/11_lnk_40,mmset1/11_lnk_13</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_14,mmset1/11_lnk_37,mmset1/11_lnk_38,mmset1/11_lnk_39,mmset1/11_lnk_40,mmset1/11_lnk_13</t>
+  </si>
+  <si>
+    <t>mmset1/11_lnk_16,mmset1/11_lnk_37,mmset1/11_lnk_38,mmset1/11_lnk_39,mmset1/11_lnk_40,mmset1/11_lnk_13</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_0,mmset1/12_lnk_11,mmset1/12_lnk_5,mmset1/12_lnk_7,mmset1/12_lnk_10,mmset1/12_lnk_2</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_9,mmset1/12_lnk_11,mmset1/12_lnk_5,mmset1/12_lnk_7,mmset1/12_lnk_10,mmset1/12_lnk_2</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_6,mmset1/12_lnk_11,mmset1/12_lnk_5,mmset1/12_lnk_7,mmset1/12_lnk_10,mmset1/12_lnk_2</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_3,mmset1/12_lnk_11,mmset1/12_lnk_5,mmset1/12_lnk_7,mmset1/12_lnk_10,mmset1/12_lnk_2</t>
+  </si>
+  <si>
+    <t>mmset1/12_lnk_4,mmset1/12_lnk_11,mmset1/12_lnk_8,mmset1/12_lnk_12,mmset1/12_lnk_13,mmset1/12_lnk_14,mmset1/12_lnk_15,mmset1/12_lnk_16,mmset1/12_lnk_17,mmset1/12_lnk_18,mmset1/12_lnk_17,mmset1/12_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/1_lnk_4,mmset4/1_lnk_3,mmset4/1_lnk_0</t>
+  </si>
+  <si>
+    <t>mmset4/1_lnk_2,mmset4/1_lnk_3</t>
+  </si>
+  <si>
+    <t>mmset4/1_lnk_1,mmset4/1_lnk_3</t>
+  </si>
+  <si>
+    <t>mmset4/2_lnk_0,mmset4/2_lnk_2,mmset4/2_lnk_1,mmset4/2_lnk_3</t>
+  </si>
+  <si>
+    <t>mmset4/2_lnk_4,mmset4/2_lnk_2</t>
+  </si>
+  <si>
+    <t>mmset4/3a_lnk_1,mmset4/3a_lnk_2,mmset4/3a_lnk_0</t>
   </si>
   <si>
     <t>mmset4/3a_lnk_3,mmset4/3a_lnk_2</t>
   </si>
   <si>
-    <t>mmset4/3b_lnk_0,mmset4/3b_lnk_1,mmset4/3b_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/3b_lnk_2,mmset4/3b_lnk_1</t>
-  </si>
-  <si>
-    <t>mmset4/3c_lnk_0,mmset4/3c_lnk_1,mmset4/3c_lnk_2</t>
-  </si>
-  <si>
-    <t>mmset4/3c_lnk_3,mmset4/3c_lnk_1</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_2,mmset4/7_lnk_11,mmset4/7_lnk_6,mmset4/7_lnk_3,mmset4/7_lnk_6</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_1,mmset4/7_lnk_15,mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_13,mmset4/7_lnk_15,mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_12,mmset4/7_lnk_15,mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_14,mmset4/7_lnk_15,mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_7,mmset4/7_lnk_15,mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_5,mmset4/7_lnk_15,mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_4,mmset4/7_lnk_15,mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_8,mmset4/7_lnk_15,mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_10,mmset4/7_lnk_15,mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_9,mmset4/7_lnk_15,mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/7_lnk_0,mmset4/7_lnk_15,mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>mmset4/8_lnk_0,mmset4/8_lnk_4,mmset4/8_lnk_2,mmset4/8_lnk_1,mmset4/8_lnk_2</t>
-  </si>
-  <si>
-    <t>mmset4/8_lnk_6,mmset4/8_lnk_8,mmset4/8_lnk_1</t>
+    <t>mmset4/3b_lnk_1,mmset4/3b_lnk_2,mmset4/3b_lnk_0</t>
+  </si>
+  <si>
+    <t>mmset4/3b_lnk_3,mmset4/3b_lnk_2</t>
+  </si>
+  <si>
+    <t>mmset4/3c_lnk_0,mmset4/3c_lnk_2,mmset4/3c_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/3c_lnk_3,mmset4/3c_lnk_2</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_6,mmset4/7_lnk_4,mmset4/7_lnk_10,mmset4/7_lnk_1,mmset4/7_lnk_10</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_14,mmset4/7_lnk_15,mmset4/7_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_7,mmset4/7_lnk_15,mmset4/7_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_3,mmset4/7_lnk_15,mmset4/7_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_9,mmset4/7_lnk_15,mmset4/7_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_0,mmset4/7_lnk_15,mmset4/7_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_5,mmset4/7_lnk_15,mmset4/7_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_13,mmset4/7_lnk_15,mmset4/7_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_12,mmset4/7_lnk_15,mmset4/7_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_8,mmset4/7_lnk_15,mmset4/7_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_2,mmset4/7_lnk_15,mmset4/7_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/7_lnk_11,mmset4/7_lnk_15,mmset4/7_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/8_lnk_7,mmset4/8_lnk_3,mmset4/8_lnk_6,mmset4/8_lnk_1,mmset4/8_lnk_6</t>
+  </si>
+  <si>
+    <t>mmset4/8_lnk_4,mmset4/8_lnk_8,mmset4/8_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/8_lnk_2,mmset4/8_lnk_8,mmset4/8_lnk_1</t>
   </si>
   <si>
     <t>mmset4/8_lnk_5,mmset4/8_lnk_8,mmset4/8_lnk_1</t>
   </si>
   <si>
-    <t>mmset4/8_lnk_7,mmset4/8_lnk_8,mmset4/8_lnk_1</t>
-  </si>
-  <si>
-    <t>mmset4/8_lnk_3,mmset4/8_lnk_8,mmset4/8_lnk_1</t>
-  </si>
-  <si>
-    <t>mmset4/11_lnk_0,mmset4/11_lnk_2,mmset4/11_lnk_1</t>
-  </si>
-  <si>
-    <t>mmset4/11_lnk_4,mmset4/11_lnk_2</t>
-  </si>
-  <si>
-    <t>mmset4/11_lnk_3,mmset4/11_lnk_2</t>
-  </si>
-  <si>
-    <t>mmset4/11_lnk_5,mmset4/11_lnk_2</t>
-  </si>
-  <si>
-    <t>mmset4/12_lnk_0,mmset4/12_lnk_2,mmset4/12_lnk_5</t>
-  </si>
-  <si>
-    <t>mmset4/12_lnk_4,mmset4/12_lnk_2</t>
-  </si>
-  <si>
-    <t>mmset4/12_lnk_3,mmset4/12_lnk_2</t>
-  </si>
-  <si>
-    <t>mmset4/12_lnk_1,mmset4/12_lnk_2</t>
-  </si>
-  <si>
-    <t>prostate/11_lnk_7,prostate/11_lnk_0,prostate/11_lnk_4,prostate/11_lnk_6</t>
-  </si>
-  <si>
-    <t>prostate/11_lnk_5,prostate/11_lnk_0</t>
-  </si>
-  <si>
-    <t>prostate/11_lnk_1,prostate/11_lnk_0</t>
-  </si>
-  <si>
-    <t>prostate/11_lnk_2,prostate/11_lnk_0</t>
-  </si>
-  <si>
-    <t>prostate/11_lnk_3,prostate/11_lnk_0</t>
-  </si>
-  <si>
-    <t>prostate/13_lnk_1,prostate/13_lnk_2,prostate/13_lnk_0</t>
-  </si>
-  <si>
-    <t>prostate/13_lnk_3,prostate/13_lnk_2</t>
-  </si>
-  <si>
-    <t>prostate/15_lnk_3,prostate/15_lnk_1,prostate/15_lnk_4,prostate/15_lnk_2</t>
-  </si>
-  <si>
-    <t>prostate/15_lnk_5,prostate/15_lnk_1</t>
-  </si>
-  <si>
-    <t>prostate/15_lnk_7,prostate/15_lnk_1</t>
-  </si>
-  <si>
-    <t>prostate/15_lnk_6,prostate/15_lnk_1</t>
-  </si>
-  <si>
-    <t>prostate/15_lnk_0,prostate/15_lnk_1</t>
-  </si>
-  <si>
-    <t>prostate/17_lnk_0,prostate/17_lnk_3,prostate/17_lnk_1</t>
-  </si>
-  <si>
-    <t>prostate/17_lnk_2,prostate/17_lnk_3</t>
-  </si>
-  <si>
-    <t>prostate/17_lnk_4,prostate/17_lnk_3</t>
-  </si>
-  <si>
-    <t>prostate/24_lnk_4,prostate/24_lnk_5,prostate/24_lnk_2</t>
-  </si>
-  <si>
-    <t>prostate/24_lnk_3,prostate/24_lnk_5</t>
-  </si>
-  <si>
-    <t>prostate/24_lnk_0,prostate/24_lnk_5</t>
+    <t>mmset4/8_lnk_0,mmset4/8_lnk_8,mmset4/8_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/11_lnk_5,mmset4/11_lnk_1,mmset4/11_lnk_4</t>
+  </si>
+  <si>
+    <t>mmset4/11_lnk_2,mmset4/11_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/11_lnk_0,mmset4/11_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/11_lnk_3,mmset4/11_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/12_lnk_5,mmset4/12_lnk_1,mmset4/12_lnk_2</t>
+  </si>
+  <si>
+    <t>mmset4/12_lnk_3,mmset4/12_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/12_lnk_0,mmset4/12_lnk_1</t>
+  </si>
+  <si>
+    <t>mmset4/12_lnk_4,mmset4/12_lnk_1</t>
+  </si>
+  <si>
+    <t>prostate/11_lnk_2,prostate/11_lnk_7,prostate/11_lnk_4,prostate/11_lnk_3</t>
+  </si>
+  <si>
+    <t>prostate/11_lnk_0,prostate/11_lnk_7</t>
+  </si>
+  <si>
+    <t>prostate/11_lnk_6,prostate/11_lnk_7</t>
+  </si>
+  <si>
+    <t>prostate/11_lnk_1,prostate/11_lnk_7</t>
+  </si>
+  <si>
+    <t>prostate/11_lnk_5,prostate/11_lnk_7</t>
+  </si>
+  <si>
+    <t>prostate/13_lnk_1,prostate/13_lnk_0,prostate/13_lnk_2</t>
+  </si>
+  <si>
+    <t>prostate/13_lnk_3,prostate/13_lnk_0</t>
+  </si>
+  <si>
+    <t>prostate/15_lnk_7,prostate/15_lnk_6,prostate/15_lnk_3,prostate/15_lnk_2</t>
+  </si>
+  <si>
+    <t>prostate/15_lnk_5,prostate/15_lnk_6</t>
+  </si>
+  <si>
+    <t>prostate/15_lnk_1,prostate/15_lnk_6</t>
+  </si>
+  <si>
+    <t>prostate/15_lnk_0,prostate/15_lnk_6</t>
+  </si>
+  <si>
+    <t>prostate/15_lnk_4,prostate/15_lnk_6</t>
+  </si>
+  <si>
+    <t>prostate/17_lnk_3,prostate/17_lnk_2,prostate/17_lnk_1</t>
+  </si>
+  <si>
+    <t>prostate/17_lnk_4,prostate/17_lnk_2</t>
+  </si>
+  <si>
+    <t>prostate/17_lnk_0,prostate/17_lnk_2</t>
+  </si>
+  <si>
+    <t>prostate/24_lnk_0,prostate/24_lnk_5,prostate/24_lnk_3</t>
+  </si>
+  <si>
+    <t>prostate/24_lnk_4,prostate/24_lnk_5</t>
+  </si>
+  <si>
+    <t>prostate/24_lnk_2,prostate/24_lnk_5</t>
   </si>
   <si>
     <t>prostate/24_lnk_1,prostate/24_lnk_5</t>
   </si>
   <si>
-    <t>prostate/26_lnk_2,prostate/26_lnk_3</t>
-  </si>
-  <si>
-    <t>prostate/26_lnk_4,prostate/26_lnk_3,prostate/26_lnk_1</t>
-  </si>
-  <si>
-    <t>prostate/26_lnk_0,prostate/26_lnk_3</t>
-  </si>
-  <si>
-    <t>prostate/26_lnk_5,prostate/26_lnk_3</t>
-  </si>
-  <si>
-    <t>semves/1_lnk_3,semves/1_lnk_1,semves/1_lnk_2,semves/1_lnk_4</t>
-  </si>
-  <si>
-    <t>semves/1_lnk_0,semves/1_lnk_1</t>
-  </si>
-  <si>
-    <t>semves/3_lnk_3,semves/3_lnk_1</t>
-  </si>
-  <si>
-    <t>semves/3_lnk_0,semves/3_lnk_1,semves/3_lnk_2</t>
-  </si>
-  <si>
-    <t>semves/5_lnk_8,semves/5_lnk_3</t>
-  </si>
-  <si>
-    <t>semves/5_lnk_2,semves/5_lnk_3,semves/5_lnk_6,semves/5_lnk_4</t>
-  </si>
-  <si>
-    <t>semves/5_lnk_0,semves/5_lnk_3</t>
-  </si>
-  <si>
-    <t>semves/5_lnk_1,semves/5_lnk_3</t>
-  </si>
-  <si>
-    <t>semves/5_lnk_5,semves/5_lnk_3</t>
-  </si>
-  <si>
-    <t>semves/5_lnk_7,semves/5_lnk_3</t>
-  </si>
-  <si>
-    <t>semves/7_lnk_1,semves/7_lnk_2,semves/7_lnk_0</t>
-  </si>
-  <si>
-    <t>semves/7_lnk_4,semves/7_lnk_2</t>
-  </si>
-  <si>
-    <t>semves/7_lnk_3,semves/7_lnk_2</t>
+    <t>prostate/26_lnk_0,prostate/26_lnk_2</t>
+  </si>
+  <si>
+    <t>prostate/26_lnk_5,prostate/26_lnk_2,prostate/26_lnk_3</t>
+  </si>
+  <si>
+    <t>prostate/26_lnk_4,prostate/26_lnk_2</t>
+  </si>
+  <si>
+    <t>prostate/26_lnk_1,prostate/26_lnk_2</t>
+  </si>
+  <si>
+    <t>semves/1_lnk_0,semves/1_lnk_4,semves/1_lnk_2,semves/1_lnk_1</t>
+  </si>
+  <si>
+    <t>semves/1_lnk_3,semves/1_lnk_4</t>
+  </si>
+  <si>
+    <t>semves/3_lnk_1,semves/3_lnk_0</t>
+  </si>
+  <si>
+    <t>semves/3_lnk_3,semves/3_lnk_0,semves/3_lnk_2</t>
+  </si>
+  <si>
+    <t>semves/5_lnk_1,semves/5_lnk_7</t>
+  </si>
+  <si>
+    <t>semves/5_lnk_5,semves/5_lnk_7,semves/5_lnk_3,semves/5_lnk_2</t>
+  </si>
+  <si>
+    <t>semves/5_lnk_6,semves/5_lnk_7</t>
+  </si>
+  <si>
+    <t>semves/5_lnk_8,semves/5_lnk_7</t>
+  </si>
+  <si>
+    <t>semves/5_lnk_4,semves/5_lnk_7</t>
+  </si>
+  <si>
+    <t>semves/5_lnk_0,semves/5_lnk_7</t>
+  </si>
+  <si>
+    <t>semves/7_lnk_4,semves/7_lnk_3,semves/7_lnk_2</t>
+  </si>
+  <si>
+    <t>semves/7_lnk_0,semves/7_lnk_3</t>
+  </si>
+  <si>
+    <t>semves/7_lnk_1,semves/7_lnk_3</t>
   </si>
   <si>
     <t>links</t>
@@ -3516,130 +3516,130 @@
     <t>Group semves/7</t>
   </si>
   <si>
-    <t>nlp:mmset1/11_lnk_18,nlp:mmset1/11_lnk_1,nlp:mmset1/11_lnk_14,nlp:mmset1/11_lnk_15,nlp:mmset1/11_lnk_29,nlp:mmset1/11_lnk_37,nlp:mmset1/11_lnk_31,nlp:mmset1/11_lnk_7,nlp:mmset1/11_lnk_11,nlp:mmset1/11_lnk_16,nlp:mmset1/11_lnk_5,nlp:mmset1/11_lnk_35,nlp:mmset1/11_lnk_4,nlp:mmset1/11_lnk_25,nlp:mmset1/11_lnk_40,nlp:mmset1/11_lnk_27,nlp:mmset1/11_lnk_8,nlp:mmset1/11_lnk_33,nlp:mmset1/11_lnk_3,nlp:mmset1/11_lnk_12,nlp:mmset1/11_lnk_2,nlp:mmset1/11_lnk_19,nlp:mmset1/11_lnk_20,nlp:mmset1/11_lnk_17,nlp:mmset1/11_lnk_9,nlp:mmset1/11_lnk_0,nlp:mmset1/11_lnk_39,nlp:mmset1/11_lnk_6,nlp:mmset1/11_lnk_38,nlp:mmset1/11_lnk_10,nlp:mmset1/11_lnk_23,nlp:mmset1/11_lnk_21,nlp:mmset1/11_lnk_13</t>
-  </si>
-  <si>
-    <t>nlp:mmset1/12_lnk_17,nlp:mmset1/12_lnk_5,nlp:mmset1/12_lnk_10,nlp:mmset1/12_lnk_15,nlp:mmset1/12_lnk_18,nlp:mmset1/12_lnk_12,nlp:mmset1/12_lnk_7,nlp:mmset1/12_lnk_1,nlp:mmset1/12_lnk_14,nlp:mmset1/12_lnk_11,nlp:mmset1/12_lnk_16,nlp:mmset1/12_lnk_3,nlp:mmset1/12_lnk_9,nlp:mmset1/12_lnk_2,nlp:mmset1/12_lnk_6,nlp:mmset1/12_lnk_4,nlp:mmset1/12_lnk_8,nlp:mmset1/12_lnk_0</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/1_lnk_0,nlp:mmset4/1_lnk_2,nlp:mmset4/1_lnk_3,nlp:mmset4/1_lnk_1,nlp:mmset4/1_lnk_4</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/2_lnk_3,nlp:mmset4/2_lnk_2,nlp:mmset4/2_lnk_0,nlp:mmset4/2_lnk_1,nlp:mmset4/2_lnk_4</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/3a_lnk_2,nlp:mmset4/3a_lnk_0,nlp:mmset4/3a_lnk_3,nlp:mmset4/3a_lnk_1</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/3b_lnk_1,nlp:mmset4/3b_lnk_0,nlp:mmset4/3b_lnk_3,nlp:mmset4/3b_lnk_2</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/3c_lnk_2,nlp:mmset4/3c_lnk_1,nlp:mmset4/3c_lnk_0,nlp:mmset4/3c_lnk_3</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/7_lnk_2,nlp:mmset4/7_lnk_9,nlp:mmset4/7_lnk_11,nlp:mmset4/7_lnk_6,nlp:mmset4/7_lnk_12,nlp:mmset4/7_lnk_10,nlp:mmset4/7_lnk_1,nlp:mmset4/7_lnk_14,nlp:mmset4/7_lnk_8,nlp:mmset4/7_lnk_13,nlp:mmset4/7_lnk_5,nlp:mmset4/7_lnk_0,nlp:mmset4/7_lnk_7,nlp:mmset4/7_lnk_4,nlp:mmset4/7_lnk_15,nlp:mmset4/7_lnk_3</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/8_lnk_8,nlp:mmset4/8_lnk_1,nlp:mmset4/8_lnk_7,nlp:mmset4/8_lnk_0,nlp:mmset4/8_lnk_3,nlp:mmset4/8_lnk_4,nlp:mmset4/8_lnk_6,nlp:mmset4/8_lnk_2,nlp:mmset4/8_lnk_5</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/11_lnk_2,nlp:mmset4/11_lnk_1,nlp:mmset4/11_lnk_0,nlp:mmset4/11_lnk_3,nlp:mmset4/11_lnk_5,nlp:mmset4/11_lnk_4</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/12_lnk_5,nlp:mmset4/12_lnk_2,nlp:mmset4/12_lnk_3,nlp:mmset4/12_lnk_4,nlp:mmset4/12_lnk_1,nlp:mmset4/12_lnk_0</t>
-  </si>
-  <si>
-    <t>nlp:prostate/11_lnk_7,nlp:prostate/11_lnk_3,nlp:prostate/11_lnk_2,nlp:prostate/11_lnk_6,nlp:prostate/11_lnk_0,nlp:prostate/11_lnk_4,nlp:prostate/11_lnk_5,nlp:prostate/11_lnk_1</t>
-  </si>
-  <si>
-    <t>nlp:prostate/13_lnk_3,nlp:prostate/13_lnk_1,nlp:prostate/13_lnk_2,nlp:prostate/13_lnk_0</t>
-  </si>
-  <si>
-    <t>nlp:prostate/15_lnk_7,nlp:prostate/15_lnk_4,nlp:prostate/15_lnk_1,nlp:prostate/15_lnk_3,nlp:prostate/15_lnk_5,nlp:prostate/15_lnk_0,nlp:prostate/15_lnk_6,nlp:prostate/15_lnk_2</t>
-  </si>
-  <si>
-    <t>nlp:prostate/17_lnk_3,nlp:prostate/17_lnk_4,nlp:prostate/17_lnk_2,nlp:prostate/17_lnk_1,nlp:prostate/17_lnk_0</t>
-  </si>
-  <si>
-    <t>nlp:prostate/24_lnk_1,nlp:prostate/24_lnk_4,nlp:prostate/24_lnk_5,nlp:prostate/24_lnk_3,nlp:prostate/24_lnk_2,nlp:prostate/24_lnk_0</t>
-  </si>
-  <si>
-    <t>nlp:prostate/26_lnk_5,nlp:prostate/26_lnk_4,nlp:prostate/26_lnk_1,nlp:prostate/26_lnk_0,nlp:prostate/26_lnk_2,nlp:prostate/26_lnk_3</t>
-  </si>
-  <si>
-    <t>nlp:semves/1_lnk_3,nlp:semves/1_lnk_2,nlp:semves/1_lnk_1,nlp:semves/1_lnk_0,nlp:semves/1_lnk_4</t>
-  </si>
-  <si>
-    <t>nlp:semves/3_lnk_0,nlp:semves/3_lnk_2,nlp:semves/3_lnk_3,nlp:semves/3_lnk_1</t>
-  </si>
-  <si>
-    <t>nlp:semves/5_lnk_7,nlp:semves/5_lnk_5,nlp:semves/5_lnk_8,nlp:semves/5_lnk_6,nlp:semves/5_lnk_4,nlp:semves/5_lnk_0,nlp:semves/5_lnk_2,nlp:semves/5_lnk_3,nlp:semves/5_lnk_1</t>
-  </si>
-  <si>
-    <t>nlp:semves/7_lnk_2,nlp:semves/7_lnk_0,nlp:semves/7_lnk_3,nlp:semves/7_lnk_4,nlp:semves/7_lnk_1</t>
-  </si>
-  <si>
-    <t>nlp:mmset1/11_n7,nlp:mmset1/11_n25,nlp:mmset1/11_n19,nlp:mmset1/11_n8,nlp:mmset1/11_n22,nlp:mmset1/11_n1,nlp:mmset1/11_n12,nlp:mmset1/11_n16,nlp:mmset1/11_n3,nlp:mmset1/11_n4,nlp:mmset1/11_n23,nlp:mmset1/11_n11,nlp:mmset1/11_n9,nlp:mmset1/11_n15,nlp:mmset1/11_n6,nlp:mmset1/11_n13,nlp:mmset1/11_n17,nlp:mmset1/11_n18,nlp:mmset1/11_n20,nlp:mmset1/11_n2,nlp:mmset1/11_n24,nlp:mmset1/11_n14,nlp:mmset1/11_n5,nlp:mmset1/11_n10</t>
-  </si>
-  <si>
-    <t>nlp:mmset1/12_n8,nlp:mmset1/12_n1,nlp:mmset1/12_n12,nlp:mmset1/12_n5,nlp:mmset1/12_n7,nlp:mmset1/12_n2,nlp:mmset1/12_n4,nlp:mmset1/12_n9,nlp:mmset1/12_n10,nlp:mmset1/12_n13,nlp:mmset1/12_n11,nlp:mmset1/12_n6,nlp:mmset1/12_n3</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/1_n1,nlp:mmset4/1_n3,nlp:mmset4/1_n6,nlp:mmset4/1_n5,nlp:mmset4/1_n4,nlp:mmset4/1_n2</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/2_n2,nlp:mmset4/2_n4,nlp:mmset4/2_n5,nlp:mmset4/2_n3,nlp:mmset4/2_n6,nlp:mmset4/2_n1</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/3a_n2,nlp:mmset4/3a_n5,nlp:mmset4/3a_n4,nlp:mmset4/3a_n1,nlp:mmset4/3a_n3</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/3b_n2,nlp:mmset4/3b_n5,nlp:mmset4/3b_n4,nlp:mmset4/3b_n1,nlp:mmset4/3b_n3</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/3c_n2,nlp:mmset4/3c_n3,nlp:mmset4/3c_n4,nlp:mmset4/3c_n5,nlp:mmset4/3c_n1</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/7_n7,nlp:mmset4/7_n3,nlp:mmset4/7_n6,nlp:mmset4/7_n10,nlp:mmset4/7_n11,nlp:mmset4/7_n5,nlp:mmset4/7_n13,nlp:mmset4/7_n15,nlp:mmset4/7_n1,nlp:mmset4/7_n2,nlp:mmset4/7_n14,nlp:mmset4/7_n8,nlp:mmset4/7_n12,nlp:mmset4/7_n4,nlp:mmset4/7_n9</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/8_n1,nlp:mmset4/8_n3,nlp:mmset4/8_n2,nlp:mmset4/8_n6,nlp:mmset4/8_n5,nlp:mmset4/8_n7,nlp:mmset4/8_n4,nlp:mmset4/8_n8</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/11_n2,nlp:mmset4/11_n4,nlp:mmset4/11_n5,nlp:mmset4/11_n6,nlp:mmset4/11_n1,nlp:mmset4/11_n3,nlp:mmset4/11_n7</t>
-  </si>
-  <si>
-    <t>nlp:mmset4/12_n5,nlp:mmset4/12_n7,nlp:mmset4/12_n1,nlp:mmset4/12_n3,nlp:mmset4/12_n4,nlp:mmset4/12_n2,nlp:mmset4/12_n6</t>
-  </si>
-  <si>
-    <t>nlp:prostate/11_n4,nlp:prostate/11_n1,nlp:prostate/11_n5,nlp:prostate/11_n9,nlp:prostate/11_n6,nlp:prostate/11_n3,nlp:prostate/11_n7,nlp:prostate/11_n2,nlp:prostate/11_n8</t>
-  </si>
-  <si>
-    <t>nlp:prostate/13_n4,nlp:prostate/13_n1,nlp:prostate/13_n2,nlp:prostate/13_n5,nlp:prostate/13_n3</t>
-  </si>
-  <si>
-    <t>nlp:prostate/15_n8,nlp:prostate/15_n7,nlp:prostate/15_n1,nlp:prostate/15_n9,nlp:prostate/15_n2,nlp:prostate/15_n6,nlp:prostate/15_n5,nlp:prostate/15_n4,nlp:prostate/15_n3</t>
-  </si>
-  <si>
-    <t>nlp:prostate/17_n5,nlp:prostate/17_n3,nlp:prostate/17_n6,nlp:prostate/17_n2,nlp:prostate/17_n1,nlp:prostate/17_n4</t>
-  </si>
-  <si>
-    <t>nlp:prostate/24_n1,nlp:prostate/24_n2,nlp:prostate/24_n3,nlp:prostate/24_n4,nlp:prostate/24_n6,nlp:prostate/24_n5,nlp:prostate/24_n7</t>
-  </si>
-  <si>
-    <t>nlp:prostate/26_n3,nlp:prostate/26_n7,nlp:prostate/26_n4,nlp:prostate/26_n1,nlp:prostate/26_n6,nlp:prostate/26_n2,nlp:prostate/26_n5</t>
-  </si>
-  <si>
-    <t>nlp:semves/1_n2,nlp:semves/1_n6,nlp:semves/1_n5,nlp:semves/1_n4,nlp:semves/1_n1,nlp:semves/1_n3</t>
-  </si>
-  <si>
-    <t>nlp:semves/3_n1,nlp:semves/3_n2,nlp:semves/3_n5,nlp:semves/3_n4,nlp:semves/3_n3</t>
-  </si>
-  <si>
-    <t>nlp:semves/5_n4,nlp:semves/5_n3,nlp:semves/5_n2,nlp:semves/5_n10,nlp:semves/5_n1,nlp:semves/5_n6,nlp:semves/5_n8,nlp:semves/5_n7,nlp:semves/5_n9,nlp:semves/5_n5</t>
-  </si>
-  <si>
-    <t>nlp:semves/7_n1,nlp:semves/7_n5,nlp:semves/7_n6,nlp:semves/7_n3,nlp:semves/7_n2,nlp:semves/7_n4</t>
+    <t>nlp:mmset1/11_lnk_21,nlp:mmset1/11_lnk_16,nlp:mmset1/11_lnk_7,nlp:mmset1/11_lnk_12,nlp:mmset1/11_lnk_8,nlp:mmset1/11_lnk_35,nlp:mmset1/11_lnk_33,nlp:mmset1/11_lnk_15,nlp:mmset1/11_lnk_10,nlp:mmset1/11_lnk_11,nlp:mmset1/11_lnk_29,nlp:mmset1/11_lnk_18,nlp:mmset1/11_lnk_14,nlp:mmset1/11_lnk_4,nlp:mmset1/11_lnk_5,nlp:mmset1/11_lnk_19,nlp:mmset1/11_lnk_3,nlp:mmset1/11_lnk_37,nlp:mmset1/11_lnk_1,nlp:mmset1/11_lnk_13,nlp:mmset1/11_lnk_9,nlp:mmset1/11_lnk_25,nlp:mmset1/11_lnk_0,nlp:mmset1/11_lnk_39,nlp:mmset1/11_lnk_2,nlp:mmset1/11_lnk_6,nlp:mmset1/11_lnk_27,nlp:mmset1/11_lnk_31,nlp:mmset1/11_lnk_38,nlp:mmset1/11_lnk_17,nlp:mmset1/11_lnk_40,nlp:mmset1/11_lnk_20,nlp:mmset1/11_lnk_23</t>
+  </si>
+  <si>
+    <t>nlp:mmset1/12_lnk_8,nlp:mmset1/12_lnk_16,nlp:mmset1/12_lnk_18,nlp:mmset1/12_lnk_0,nlp:mmset1/12_lnk_10,nlp:mmset1/12_lnk_17,nlp:mmset1/12_lnk_6,nlp:mmset1/12_lnk_9,nlp:mmset1/12_lnk_11,nlp:mmset1/12_lnk_12,nlp:mmset1/12_lnk_1,nlp:mmset1/12_lnk_3,nlp:mmset1/12_lnk_2,nlp:mmset1/12_lnk_5,nlp:mmset1/12_lnk_7,nlp:mmset1/12_lnk_14,nlp:mmset1/12_lnk_4,nlp:mmset1/12_lnk_15</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/1_lnk_3,nlp:mmset4/1_lnk_0,nlp:mmset4/1_lnk_4,nlp:mmset4/1_lnk_1,nlp:mmset4/1_lnk_2</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/2_lnk_3,nlp:mmset4/2_lnk_0,nlp:mmset4/2_lnk_4,nlp:mmset4/2_lnk_2,nlp:mmset4/2_lnk_1</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/3a_lnk_3,nlp:mmset4/3a_lnk_0,nlp:mmset4/3a_lnk_2,nlp:mmset4/3a_lnk_1</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/3b_lnk_2,nlp:mmset4/3b_lnk_3,nlp:mmset4/3b_lnk_1,nlp:mmset4/3b_lnk_0</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/3c_lnk_3,nlp:mmset4/3c_lnk_1,nlp:mmset4/3c_lnk_2,nlp:mmset4/3c_lnk_0</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/7_lnk_12,nlp:mmset4/7_lnk_6,nlp:mmset4/7_lnk_7,nlp:mmset4/7_lnk_4,nlp:mmset4/7_lnk_0,nlp:mmset4/7_lnk_1,nlp:mmset4/7_lnk_8,nlp:mmset4/7_lnk_5,nlp:mmset4/7_lnk_9,nlp:mmset4/7_lnk_10,nlp:mmset4/7_lnk_15,nlp:mmset4/7_lnk_3,nlp:mmset4/7_lnk_11,nlp:mmset4/7_lnk_14,nlp:mmset4/7_lnk_13,nlp:mmset4/7_lnk_2</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/8_lnk_4,nlp:mmset4/8_lnk_8,nlp:mmset4/8_lnk_0,nlp:mmset4/8_lnk_7,nlp:mmset4/8_lnk_3,nlp:mmset4/8_lnk_6,nlp:mmset4/8_lnk_1,nlp:mmset4/8_lnk_2,nlp:mmset4/8_lnk_5</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/11_lnk_1,nlp:mmset4/11_lnk_4,nlp:mmset4/11_lnk_0,nlp:mmset4/11_lnk_2,nlp:mmset4/11_lnk_3,nlp:mmset4/11_lnk_5</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/12_lnk_5,nlp:mmset4/12_lnk_2,nlp:mmset4/12_lnk_3,nlp:mmset4/12_lnk_1,nlp:mmset4/12_lnk_4,nlp:mmset4/12_lnk_0</t>
+  </si>
+  <si>
+    <t>nlp:prostate/11_lnk_1,nlp:prostate/11_lnk_3,nlp:prostate/11_lnk_0,nlp:prostate/11_lnk_5,nlp:prostate/11_lnk_6,nlp:prostate/11_lnk_2,nlp:prostate/11_lnk_7,nlp:prostate/11_lnk_4</t>
+  </si>
+  <si>
+    <t>nlp:prostate/13_lnk_1,nlp:prostate/13_lnk_2,nlp:prostate/13_lnk_3,nlp:prostate/13_lnk_0</t>
+  </si>
+  <si>
+    <t>nlp:prostate/15_lnk_3,nlp:prostate/15_lnk_5,nlp:prostate/15_lnk_7,nlp:prostate/15_lnk_6,nlp:prostate/15_lnk_1,nlp:prostate/15_lnk_2,nlp:prostate/15_lnk_4,nlp:prostate/15_lnk_0</t>
+  </si>
+  <si>
+    <t>nlp:prostate/17_lnk_3,nlp:prostate/17_lnk_4,nlp:prostate/17_lnk_0,nlp:prostate/17_lnk_2,nlp:prostate/17_lnk_1</t>
+  </si>
+  <si>
+    <t>nlp:prostate/24_lnk_3,nlp:prostate/24_lnk_5,nlp:prostate/24_lnk_0,nlp:prostate/24_lnk_4,nlp:prostate/24_lnk_1,nlp:prostate/24_lnk_2</t>
+  </si>
+  <si>
+    <t>nlp:prostate/26_lnk_1,nlp:prostate/26_lnk_2,nlp:prostate/26_lnk_5,nlp:prostate/26_lnk_4,nlp:prostate/26_lnk_0,nlp:prostate/26_lnk_3</t>
+  </si>
+  <si>
+    <t>nlp:semves/1_lnk_1,nlp:semves/1_lnk_3,nlp:semves/1_lnk_0,nlp:semves/1_lnk_2,nlp:semves/1_lnk_4</t>
+  </si>
+  <si>
+    <t>nlp:semves/3_lnk_2,nlp:semves/3_lnk_3,nlp:semves/3_lnk_1,nlp:semves/3_lnk_0</t>
+  </si>
+  <si>
+    <t>nlp:semves/5_lnk_7,nlp:semves/5_lnk_3,nlp:semves/5_lnk_1,nlp:semves/5_lnk_5,nlp:semves/5_lnk_6,nlp:semves/5_lnk_0,nlp:semves/5_lnk_8,nlp:semves/5_lnk_4,nlp:semves/5_lnk_2</t>
+  </si>
+  <si>
+    <t>nlp:semves/7_lnk_1,nlp:semves/7_lnk_2,nlp:semves/7_lnk_4,nlp:semves/7_lnk_0,nlp:semves/7_lnk_3</t>
+  </si>
+  <si>
+    <t>nlp:mmset1/11_n20,nlp:mmset1/11_n5,nlp:mmset1/11_n13,nlp:mmset1/11_n4,nlp:mmset1/11_n2,nlp:mmset1/11_n14,nlp:mmset1/11_n24,nlp:mmset1/11_n17,nlp:mmset1/11_n15,nlp:mmset1/11_n23,nlp:mmset1/11_n19,nlp:mmset1/11_n8,nlp:mmset1/11_n6,nlp:mmset1/11_n16,nlp:mmset1/11_n10,nlp:mmset1/11_n3,nlp:mmset1/11_n22,nlp:mmset1/11_n11,nlp:mmset1/11_n25,nlp:mmset1/11_n1,nlp:mmset1/11_n9,nlp:mmset1/11_n18,nlp:mmset1/11_n12,nlp:mmset1/11_n7</t>
+  </si>
+  <si>
+    <t>nlp:mmset1/12_n10,nlp:mmset1/12_n3,nlp:mmset1/12_n8,nlp:mmset1/12_n4,nlp:mmset1/12_n2,nlp:mmset1/12_n1,nlp:mmset1/12_n11,nlp:mmset1/12_n12,nlp:mmset1/12_n7,nlp:mmset1/12_n9,nlp:mmset1/12_n13,nlp:mmset1/12_n5,nlp:mmset1/12_n6</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/1_n1,nlp:mmset4/1_n5,nlp:mmset4/1_n3,nlp:mmset4/1_n6,nlp:mmset4/1_n2,nlp:mmset4/1_n4</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/2_n3,nlp:mmset4/2_n6,nlp:mmset4/2_n5,nlp:mmset4/2_n1,nlp:mmset4/2_n4,nlp:mmset4/2_n2</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/3a_n1,nlp:mmset4/3a_n5,nlp:mmset4/3a_n3,nlp:mmset4/3a_n4,nlp:mmset4/3a_n2</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/3b_n2,nlp:mmset4/3b_n5,nlp:mmset4/3b_n1,nlp:mmset4/3b_n4,nlp:mmset4/3b_n3</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/3c_n2,nlp:mmset4/3c_n3,nlp:mmset4/3c_n5,nlp:mmset4/3c_n4,nlp:mmset4/3c_n1</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/7_n10,nlp:mmset4/7_n4,nlp:mmset4/7_n2,nlp:mmset4/7_n15,nlp:mmset4/7_n1,nlp:mmset4/7_n12,nlp:mmset4/7_n14,nlp:mmset4/7_n13,nlp:mmset4/7_n9,nlp:mmset4/7_n3,nlp:mmset4/7_n6,nlp:mmset4/7_n7,nlp:mmset4/7_n5,nlp:mmset4/7_n11,nlp:mmset4/7_n8</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/8_n5,nlp:mmset4/8_n3,nlp:mmset4/8_n6,nlp:mmset4/8_n7,nlp:mmset4/8_n2,nlp:mmset4/8_n1,nlp:mmset4/8_n4,nlp:mmset4/8_n8</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/11_n4,nlp:mmset4/11_n1,nlp:mmset4/11_n2,nlp:mmset4/11_n3,nlp:mmset4/11_n5,nlp:mmset4/11_n7,nlp:mmset4/11_n6</t>
+  </si>
+  <si>
+    <t>nlp:mmset4/12_n1,nlp:mmset4/12_n3,nlp:mmset4/12_n4,nlp:mmset4/12_n7,nlp:mmset4/12_n2,nlp:mmset4/12_n5,nlp:mmset4/12_n6</t>
+  </si>
+  <si>
+    <t>nlp:prostate/11_n3,nlp:prostate/11_n2,nlp:prostate/11_n9,nlp:prostate/11_n5,nlp:prostate/11_n8,nlp:prostate/11_n1,nlp:prostate/11_n6,nlp:prostate/11_n4,nlp:prostate/11_n7</t>
+  </si>
+  <si>
+    <t>nlp:prostate/13_n2,nlp:prostate/13_n4,nlp:prostate/13_n5,nlp:prostate/13_n3,nlp:prostate/13_n1</t>
+  </si>
+  <si>
+    <t>nlp:prostate/15_n2,nlp:prostate/15_n4,nlp:prostate/15_n3,nlp:prostate/15_n5,nlp:prostate/15_n7,nlp:prostate/15_n8,nlp:prostate/15_n1,nlp:prostate/15_n6,nlp:prostate/15_n9</t>
+  </si>
+  <si>
+    <t>nlp:prostate/17_n1,nlp:prostate/17_n6,nlp:prostate/17_n4,nlp:prostate/17_n3,nlp:prostate/17_n5,nlp:prostate/17_n2</t>
+  </si>
+  <si>
+    <t>nlp:prostate/24_n5,nlp:prostate/24_n2,nlp:prostate/24_n1,nlp:prostate/24_n4,nlp:prostate/24_n6,nlp:prostate/24_n3,nlp:prostate/24_n7</t>
+  </si>
+  <si>
+    <t>nlp:prostate/26_n2,nlp:prostate/26_n7,nlp:prostate/26_n1,nlp:prostate/26_n3,nlp:prostate/26_n5,nlp:prostate/26_n4,nlp:prostate/26_n6</t>
+  </si>
+  <si>
+    <t>nlp:semves/1_n4,nlp:semves/1_n5,nlp:semves/1_n2,nlp:semves/1_n6,nlp:semves/1_n3,nlp:semves/1_n1</t>
+  </si>
+  <si>
+    <t>nlp:semves/3_n4,nlp:semves/3_n5,nlp:semves/3_n1,nlp:semves/3_n2,nlp:semves/3_n3</t>
+  </si>
+  <si>
+    <t>nlp:semves/5_n2,nlp:semves/5_n9,nlp:semves/5_n6,nlp:semves/5_n10,nlp:semves/5_n5,nlp:semves/5_n7,nlp:semves/5_n8,nlp:semves/5_n4,nlp:semves/5_n3,nlp:semves/5_n1</t>
+  </si>
+  <si>
+    <t>nlp:semves/7_n6,nlp:semves/7_n4,nlp:semves/7_n5,nlp:semves/7_n1,nlp:semves/7_n3,nlp:semves/7_n2</t>
   </si>
   <si>
     <t>prefix</t>
@@ -5825,7 +5825,7 @@
         <v>488</v>
       </c>
       <c r="E2" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5836,13 +5836,13 @@
         <v>417</v>
       </c>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D3" t="s">
         <v>489</v>
       </c>
       <c r="E3" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5859,7 +5859,7 @@
         <v>490</v>
       </c>
       <c r="E4" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5876,7 +5876,7 @@
         <v>490</v>
       </c>
       <c r="E5" t="s">
-        <v>631</v>
+        <v>499</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -5884,16 +5884,16 @@
         <v>250</v>
       </c>
       <c r="B6" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C6" t="s">
         <v>239</v>
       </c>
       <c r="D6" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="E6" t="s">
-        <v>632</v>
+        <v>496</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5901,16 +5901,16 @@
         <v>251</v>
       </c>
       <c r="B7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C7" t="s">
         <v>239</v>
       </c>
       <c r="D7" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="E7" t="s">
-        <v>633</v>
+        <v>497</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5918,16 +5918,16 @@
         <v>252</v>
       </c>
       <c r="B8" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C8" t="s">
         <v>239</v>
       </c>
       <c r="D8" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="E8" t="s">
-        <v>634</v>
+        <v>496</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5935,16 +5935,16 @@
         <v>253</v>
       </c>
       <c r="B9" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C9" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D9" t="s">
+        <v>492</v>
+      </c>
+      <c r="E9" t="s">
         <v>491</v>
-      </c>
-      <c r="E9" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5952,16 +5952,16 @@
         <v>254</v>
       </c>
       <c r="B10" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D10" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="E10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5969,16 +5969,16 @@
         <v>255</v>
       </c>
       <c r="B11" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D11" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="E11" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -5986,16 +5986,16 @@
         <v>256</v>
       </c>
       <c r="B12" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D12" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E12" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -6003,16 +6003,16 @@
         <v>257</v>
       </c>
       <c r="B13" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C13" t="s">
         <v>239</v>
       </c>
       <c r="D13" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E13" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -6020,16 +6020,16 @@
         <v>258</v>
       </c>
       <c r="B14" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C14" t="s">
         <v>239</v>
       </c>
       <c r="D14" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E14" t="s">
-        <v>490</v>
+        <v>631</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -6043,10 +6043,10 @@
         <v>239</v>
       </c>
       <c r="D15" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E15" t="s">
-        <v>494</v>
+        <v>632</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -6060,10 +6060,10 @@
         <v>239</v>
       </c>
       <c r="D16" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E16" t="s">
-        <v>499</v>
+        <v>633</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6071,16 +6071,16 @@
         <v>261</v>
       </c>
       <c r="B17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D17" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E17" t="s">
-        <v>490</v>
+        <v>634</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6088,16 +6088,16 @@
         <v>262</v>
       </c>
       <c r="B18" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C18" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D18" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E18" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -6105,16 +6105,16 @@
         <v>263</v>
       </c>
       <c r="B19" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C19" t="s">
         <v>239</v>
       </c>
       <c r="D19" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="E19" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -6122,16 +6122,16 @@
         <v>264</v>
       </c>
       <c r="B20" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C20" t="s">
         <v>239</v>
       </c>
       <c r="D20" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="E20" t="s">
-        <v>635</v>
+        <v>491</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -6145,10 +6145,10 @@
         <v>239</v>
       </c>
       <c r="D21" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="E21" t="s">
-        <v>636</v>
+        <v>496</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -6162,10 +6162,10 @@
         <v>239</v>
       </c>
       <c r="D22" t="s">
+        <v>497</v>
+      </c>
+      <c r="E22" t="s">
         <v>490</v>
-      </c>
-      <c r="E22" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -6173,16 +6173,16 @@
         <v>267</v>
       </c>
       <c r="B23" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D23" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
       <c r="E23" t="s">
-        <v>638</v>
+        <v>492</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -6190,16 +6190,16 @@
         <v>268</v>
       </c>
       <c r="B24" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C24" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D24" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E24" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -6207,16 +6207,16 @@
         <v>269</v>
       </c>
       <c r="B25" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D25" t="s">
-        <v>490</v>
+        <v>500</v>
       </c>
       <c r="E25" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -6224,16 +6224,16 @@
         <v>270</v>
       </c>
       <c r="B26" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C26" t="s">
         <v>239</v>
       </c>
       <c r="D26" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="E26" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -6241,16 +6241,16 @@
         <v>271</v>
       </c>
       <c r="B27" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C27" t="s">
         <v>239</v>
       </c>
       <c r="D27" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="E27" t="s">
-        <v>494</v>
+        <v>635</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -6258,16 +6258,16 @@
         <v>272</v>
       </c>
       <c r="B28" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C28" t="s">
         <v>239</v>
       </c>
       <c r="D28" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="E28" t="s">
-        <v>497</v>
+        <v>636</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -6278,13 +6278,13 @@
         <v>431</v>
       </c>
       <c r="C29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D29" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="E29" t="s">
-        <v>488</v>
+        <v>637</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -6292,16 +6292,16 @@
         <v>274</v>
       </c>
       <c r="B30" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C30" t="s">
         <v>239</v>
       </c>
       <c r="D30" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="E30" t="s">
-        <v>494</v>
+        <v>638</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -6312,13 +6312,13 @@
         <v>432</v>
       </c>
       <c r="C31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D31" t="s">
         <v>501</v>
       </c>
       <c r="E31" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -6335,7 +6335,7 @@
         <v>502</v>
       </c>
       <c r="E32" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -6346,13 +6346,13 @@
         <v>434</v>
       </c>
       <c r="C33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D33" t="s">
-        <v>490</v>
+        <v>503</v>
       </c>
       <c r="E33" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -6363,13 +6363,13 @@
         <v>435</v>
       </c>
       <c r="C34" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D34" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="E34" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -6386,7 +6386,7 @@
         <v>504</v>
       </c>
       <c r="E35" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -6397,13 +6397,13 @@
         <v>436</v>
       </c>
       <c r="C36" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D36" t="s">
         <v>505</v>
       </c>
       <c r="E36" t="s">
-        <v>510</v>
+        <v>639</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -6411,7 +6411,7 @@
         <v>281</v>
       </c>
       <c r="B37" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C37" t="s">
         <v>239</v>
@@ -6420,7 +6420,7 @@
         <v>505</v>
       </c>
       <c r="E37" t="s">
-        <v>507</v>
+        <v>640</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -6428,16 +6428,16 @@
         <v>282</v>
       </c>
       <c r="B38" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="C38" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D38" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E38" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -6445,16 +6445,16 @@
         <v>283</v>
       </c>
       <c r="B39" t="s">
-        <v>437</v>
+        <v>417</v>
       </c>
       <c r="C39" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D39" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E39" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -6462,16 +6462,16 @@
         <v>284</v>
       </c>
       <c r="B40" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="C40" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D40" t="s">
         <v>507</v>
       </c>
       <c r="E40" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -6479,16 +6479,16 @@
         <v>285</v>
       </c>
       <c r="B41" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C41" t="s">
         <v>239</v>
       </c>
       <c r="D41" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E41" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -6496,16 +6496,16 @@
         <v>286</v>
       </c>
       <c r="B42" t="s">
-        <v>422</v>
+        <v>438</v>
       </c>
       <c r="C42" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D42" t="s">
         <v>508</v>
       </c>
       <c r="E42" t="s">
-        <v>509</v>
+        <v>641</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -6513,16 +6513,16 @@
         <v>287</v>
       </c>
       <c r="B43" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="C43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D43" t="s">
         <v>509</v>
       </c>
       <c r="E43" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -6556,7 +6556,7 @@
         <v>510</v>
       </c>
       <c r="E45" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -6564,16 +6564,16 @@
         <v>290</v>
       </c>
       <c r="B46" t="s">
-        <v>425</v>
+        <v>440</v>
       </c>
       <c r="C46" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D46" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="E46" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -6587,10 +6587,10 @@
         <v>239</v>
       </c>
       <c r="D47" t="s">
+        <v>508</v>
+      </c>
+      <c r="E47" t="s">
         <v>512</v>
-      </c>
-      <c r="E47" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -6604,10 +6604,10 @@
         <v>239</v>
       </c>
       <c r="D48" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="E48" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -6615,16 +6615,16 @@
         <v>293</v>
       </c>
       <c r="B49" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="C49" t="s">
         <v>238</v>
       </c>
       <c r="D49" t="s">
+        <v>511</v>
+      </c>
+      <c r="E49" t="s">
         <v>513</v>
-      </c>
-      <c r="E49" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -6638,7 +6638,7 @@
         <v>239</v>
       </c>
       <c r="D50" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="E50" t="s">
         <v>505</v>
@@ -6655,10 +6655,10 @@
         <v>239</v>
       </c>
       <c r="D51" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="E51" t="s">
-        <v>640</v>
+        <v>508</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -6669,13 +6669,13 @@
         <v>442</v>
       </c>
       <c r="C52" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D52" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E52" t="s">
-        <v>641</v>
+        <v>508</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -6709,7 +6709,7 @@
         <v>515</v>
       </c>
       <c r="E54" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -6720,13 +6720,13 @@
         <v>444</v>
       </c>
       <c r="C55" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D55" t="s">
         <v>516</v>
       </c>
       <c r="E55" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -6737,13 +6737,13 @@
         <v>445</v>
       </c>
       <c r="C56" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D56" t="s">
         <v>517</v>
       </c>
       <c r="E56" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -6760,7 +6760,7 @@
         <v>518</v>
       </c>
       <c r="E57" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -6771,13 +6771,13 @@
         <v>447</v>
       </c>
       <c r="C58" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D58" t="s">
         <v>519</v>
       </c>
       <c r="E58" t="s">
-        <v>643</v>
+        <v>521</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -6785,10 +6785,10 @@
         <v>303</v>
       </c>
       <c r="B59" t="s">
-        <v>448</v>
+        <v>227</v>
       </c>
       <c r="C59" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D59" t="s">
         <v>520</v>
@@ -6802,16 +6802,16 @@
         <v>304</v>
       </c>
       <c r="B60" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C60" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D60" t="s">
         <v>521</v>
       </c>
       <c r="E60" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -6819,16 +6819,16 @@
         <v>305</v>
       </c>
       <c r="B61" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="C61" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D61" t="s">
         <v>522</v>
       </c>
       <c r="E61" t="s">
-        <v>523</v>
+        <v>643</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -6836,16 +6836,16 @@
         <v>306</v>
       </c>
       <c r="B62" t="s">
-        <v>227</v>
+        <v>449</v>
       </c>
       <c r="C62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D62" t="s">
         <v>523</v>
       </c>
       <c r="E62" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -6853,16 +6853,16 @@
         <v>307</v>
       </c>
       <c r="B63" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="C63" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D63" t="s">
         <v>524</v>
       </c>
       <c r="E63" t="s">
-        <v>526</v>
+        <v>644</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -6870,16 +6870,16 @@
         <v>308</v>
       </c>
       <c r="B64" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="C64" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D64" t="s">
         <v>525</v>
       </c>
       <c r="E64" t="s">
-        <v>644</v>
+        <v>526</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -6896,7 +6896,7 @@
         <v>526</v>
       </c>
       <c r="E65" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -6904,7 +6904,7 @@
         <v>310</v>
       </c>
       <c r="B66" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C66" t="s">
         <v>238</v>
@@ -6921,16 +6921,16 @@
         <v>311</v>
       </c>
       <c r="B67" t="s">
-        <v>227</v>
+        <v>450</v>
       </c>
       <c r="C67" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D67" t="s">
         <v>528</v>
       </c>
       <c r="E67" t="s">
-        <v>529</v>
+        <v>645</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -6938,16 +6938,16 @@
         <v>312</v>
       </c>
       <c r="B68" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="C68" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D68" t="s">
         <v>529</v>
       </c>
       <c r="E68" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -6955,16 +6955,16 @@
         <v>313</v>
       </c>
       <c r="B69" t="s">
-        <v>447</v>
+        <v>211</v>
       </c>
       <c r="C69" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D69" t="s">
         <v>530</v>
       </c>
       <c r="E69" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -6972,16 +6972,16 @@
         <v>314</v>
       </c>
       <c r="B70" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C70" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D70" t="s">
         <v>531</v>
       </c>
       <c r="E70" t="s">
-        <v>645</v>
+        <v>530</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -6998,7 +6998,7 @@
         <v>532</v>
       </c>
       <c r="E71" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -7006,16 +7006,16 @@
         <v>316</v>
       </c>
       <c r="B72" t="s">
-        <v>211</v>
+        <v>451</v>
       </c>
       <c r="C72" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D72" t="s">
         <v>533</v>
       </c>
       <c r="E72" t="s">
-        <v>534</v>
+        <v>646</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -7023,16 +7023,16 @@
         <v>317</v>
       </c>
       <c r="B73" t="s">
-        <v>451</v>
+        <v>211</v>
       </c>
       <c r="C73" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D73" t="s">
         <v>534</v>
       </c>
       <c r="E73" t="s">
-        <v>646</v>
+        <v>533</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -7040,7 +7040,7 @@
         <v>318</v>
       </c>
       <c r="B74" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C74" t="s">
         <v>238</v>
@@ -7049,7 +7049,7 @@
         <v>535</v>
       </c>
       <c r="E74" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -7066,7 +7066,7 @@
         <v>536</v>
       </c>
       <c r="E75" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -7074,16 +7074,16 @@
         <v>320</v>
       </c>
       <c r="B76" t="s">
-        <v>421</v>
+        <v>453</v>
       </c>
       <c r="C76" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D76" t="s">
         <v>537</v>
       </c>
       <c r="E76" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -7091,7 +7091,7 @@
         <v>321</v>
       </c>
       <c r="B77" t="s">
-        <v>419</v>
+        <v>454</v>
       </c>
       <c r="C77" t="s">
         <v>238</v>
@@ -7100,7 +7100,7 @@
         <v>538</v>
       </c>
       <c r="E77" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -7108,16 +7108,16 @@
         <v>322</v>
       </c>
       <c r="B78" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="C78" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D78" t="s">
         <v>539</v>
       </c>
       <c r="E78" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -7125,16 +7125,16 @@
         <v>323</v>
       </c>
       <c r="B79" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C79" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D79" t="s">
         <v>540</v>
       </c>
       <c r="E79" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -7142,16 +7142,16 @@
         <v>324</v>
       </c>
       <c r="B80" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C80" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D80" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E80" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -7159,16 +7159,16 @@
         <v>325</v>
       </c>
       <c r="B81" t="s">
-        <v>224</v>
+        <v>457</v>
       </c>
       <c r="C81" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D81" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E81" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -7176,16 +7176,16 @@
         <v>326</v>
       </c>
       <c r="B82" t="s">
-        <v>456</v>
+        <v>428</v>
       </c>
       <c r="C82" t="s">
         <v>238</v>
       </c>
       <c r="D82" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E82" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -7193,16 +7193,16 @@
         <v>327</v>
       </c>
       <c r="B83" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
       <c r="C83" t="s">
         <v>238</v>
       </c>
       <c r="D83" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E83" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -7216,10 +7216,10 @@
         <v>238</v>
       </c>
       <c r="D84" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E84" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -7233,10 +7233,10 @@
         <v>238</v>
       </c>
       <c r="D85" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E85" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -7244,16 +7244,16 @@
         <v>330</v>
       </c>
       <c r="B86" t="s">
-        <v>460</v>
+        <v>224</v>
       </c>
       <c r="C86" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D86" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E86" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -7264,13 +7264,13 @@
         <v>460</v>
       </c>
       <c r="C87" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D87" t="s">
         <v>547</v>
       </c>
       <c r="E87" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -7287,7 +7287,7 @@
         <v>548</v>
       </c>
       <c r="E88" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -7295,7 +7295,7 @@
         <v>333</v>
       </c>
       <c r="B89" t="s">
-        <v>435</v>
+        <v>462</v>
       </c>
       <c r="C89" t="s">
         <v>238</v>
@@ -7304,7 +7304,7 @@
         <v>549</v>
       </c>
       <c r="E89" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -7312,7 +7312,7 @@
         <v>334</v>
       </c>
       <c r="B90" t="s">
-        <v>462</v>
+        <v>430</v>
       </c>
       <c r="C90" t="s">
         <v>238</v>
@@ -7321,7 +7321,7 @@
         <v>550</v>
       </c>
       <c r="E90" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -7329,7 +7329,7 @@
         <v>335</v>
       </c>
       <c r="B91" t="s">
-        <v>421</v>
+        <v>452</v>
       </c>
       <c r="C91" t="s">
         <v>238</v>
@@ -7338,7 +7338,7 @@
         <v>551</v>
       </c>
       <c r="E91" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -7355,7 +7355,7 @@
         <v>552</v>
       </c>
       <c r="E92" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -7363,16 +7363,16 @@
         <v>337</v>
       </c>
       <c r="B93" t="s">
-        <v>224</v>
+        <v>455</v>
       </c>
       <c r="C93" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D93" t="s">
         <v>553</v>
       </c>
       <c r="E93" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -7383,13 +7383,13 @@
         <v>456</v>
       </c>
       <c r="C94" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D94" t="s">
         <v>554</v>
       </c>
       <c r="E94" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -7397,16 +7397,16 @@
         <v>339</v>
       </c>
       <c r="B95" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C95" t="s">
         <v>239</v>
       </c>
       <c r="D95" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E95" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -7414,16 +7414,16 @@
         <v>340</v>
       </c>
       <c r="B96" t="s">
-        <v>460</v>
+        <v>432</v>
       </c>
       <c r="C96" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D96" t="s">
         <v>555</v>
       </c>
       <c r="E96" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -7431,7 +7431,7 @@
         <v>341</v>
       </c>
       <c r="B97" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C97" t="s">
         <v>238</v>
@@ -7440,7 +7440,7 @@
         <v>556</v>
       </c>
       <c r="E97" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -7448,16 +7448,16 @@
         <v>342</v>
       </c>
       <c r="B98" t="s">
-        <v>435</v>
+        <v>224</v>
       </c>
       <c r="C98" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D98" t="s">
         <v>557</v>
       </c>
       <c r="E98" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -7465,7 +7465,7 @@
         <v>343</v>
       </c>
       <c r="B99" t="s">
-        <v>462</v>
+        <v>430</v>
       </c>
       <c r="C99" t="s">
         <v>238</v>
@@ -7474,7 +7474,7 @@
         <v>558</v>
       </c>
       <c r="E99" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -7482,7 +7482,7 @@
         <v>344</v>
       </c>
       <c r="B100" t="s">
-        <v>421</v>
+        <v>455</v>
       </c>
       <c r="C100" t="s">
         <v>238</v>
@@ -7491,7 +7491,7 @@
         <v>559</v>
       </c>
       <c r="E100" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -7499,16 +7499,16 @@
         <v>345</v>
       </c>
       <c r="B101" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="C101" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D101" t="s">
         <v>560</v>
       </c>
       <c r="E101" t="s">
-        <v>647</v>
+        <v>563</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -7516,10 +7516,10 @@
         <v>346</v>
       </c>
       <c r="B102" t="s">
-        <v>460</v>
+        <v>432</v>
       </c>
       <c r="C102" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D102" t="s">
         <v>561</v>
@@ -7533,7 +7533,7 @@
         <v>347</v>
       </c>
       <c r="B103" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C103" t="s">
         <v>238</v>
@@ -7542,7 +7542,7 @@
         <v>562</v>
       </c>
       <c r="E103" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -7550,16 +7550,16 @@
         <v>348</v>
       </c>
       <c r="B104" t="s">
-        <v>435</v>
+        <v>463</v>
       </c>
       <c r="C104" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D104" t="s">
         <v>563</v>
       </c>
       <c r="E104" t="s">
-        <v>561</v>
+        <v>647</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -7567,7 +7567,7 @@
         <v>349</v>
       </c>
       <c r="B105" t="s">
-        <v>462</v>
+        <v>430</v>
       </c>
       <c r="C105" t="s">
         <v>238</v>
@@ -7576,7 +7576,7 @@
         <v>564</v>
       </c>
       <c r="E105" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -7584,7 +7584,7 @@
         <v>350</v>
       </c>
       <c r="B106" t="s">
-        <v>421</v>
+        <v>455</v>
       </c>
       <c r="C106" t="s">
         <v>238</v>
@@ -7593,7 +7593,7 @@
         <v>565</v>
       </c>
       <c r="E106" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -7601,10 +7601,10 @@
         <v>351</v>
       </c>
       <c r="B107" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="C107" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D107" t="s">
         <v>566</v>
@@ -7618,16 +7618,16 @@
         <v>352</v>
       </c>
       <c r="B108" t="s">
-        <v>460</v>
+        <v>188</v>
       </c>
       <c r="C108" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D108" t="s">
         <v>567</v>
       </c>
       <c r="E108" t="s">
-        <v>570</v>
+        <v>648</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -7635,7 +7635,7 @@
         <v>353</v>
       </c>
       <c r="B109" t="s">
-        <v>461</v>
+        <v>432</v>
       </c>
       <c r="C109" t="s">
         <v>238</v>
@@ -7644,7 +7644,7 @@
         <v>568</v>
       </c>
       <c r="E109" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -7652,7 +7652,7 @@
         <v>354</v>
       </c>
       <c r="B110" t="s">
-        <v>435</v>
+        <v>459</v>
       </c>
       <c r="C110" t="s">
         <v>238</v>
@@ -7661,7 +7661,7 @@
         <v>569</v>
       </c>
       <c r="E110" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -7669,16 +7669,16 @@
         <v>355</v>
       </c>
       <c r="B111" t="s">
-        <v>188</v>
+        <v>430</v>
       </c>
       <c r="C111" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D111" t="s">
         <v>570</v>
       </c>
       <c r="E111" t="s">
-        <v>648</v>
+        <v>566</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -7686,16 +7686,16 @@
         <v>356</v>
       </c>
       <c r="B112" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="C112" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D112" t="s">
         <v>571</v>
       </c>
       <c r="E112" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -7703,7 +7703,7 @@
         <v>357</v>
       </c>
       <c r="B113" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="C113" t="s">
         <v>238</v>
@@ -7712,7 +7712,7 @@
         <v>572</v>
       </c>
       <c r="E113" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -7720,7 +7720,7 @@
         <v>358</v>
       </c>
       <c r="B114" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="C114" t="s">
         <v>238</v>
@@ -7729,7 +7729,7 @@
         <v>573</v>
       </c>
       <c r="E114" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -7737,16 +7737,16 @@
         <v>359</v>
       </c>
       <c r="B115" t="s">
-        <v>466</v>
+        <v>227</v>
       </c>
       <c r="C115" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D115" t="s">
         <v>574</v>
       </c>
       <c r="E115" t="s">
-        <v>571</v>
+        <v>649</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -7763,7 +7763,7 @@
         <v>575</v>
       </c>
       <c r="E116" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -7771,7 +7771,7 @@
         <v>361</v>
       </c>
       <c r="B117" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="C117" t="s">
         <v>238</v>
@@ -7780,7 +7780,7 @@
         <v>576</v>
       </c>
       <c r="E117" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -7788,16 +7788,16 @@
         <v>362</v>
       </c>
       <c r="B118" t="s">
-        <v>227</v>
+        <v>460</v>
       </c>
       <c r="C118" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D118" t="s">
         <v>577</v>
       </c>
       <c r="E118" t="s">
-        <v>649</v>
+        <v>578</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -7805,16 +7805,16 @@
         <v>363</v>
       </c>
       <c r="B119" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="C119" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D119" t="s">
         <v>578</v>
       </c>
       <c r="E119" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -7822,16 +7822,16 @@
         <v>364</v>
       </c>
       <c r="B120" t="s">
-        <v>227</v>
+        <v>445</v>
       </c>
       <c r="C120" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D120" t="s">
         <v>579</v>
       </c>
       <c r="E120" t="s">
-        <v>650</v>
+        <v>581</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -7848,7 +7848,7 @@
         <v>580</v>
       </c>
       <c r="E121" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -7856,16 +7856,16 @@
         <v>366</v>
       </c>
       <c r="B122" t="s">
-        <v>444</v>
+        <v>227</v>
       </c>
       <c r="C122" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D122" t="s">
         <v>581</v>
       </c>
       <c r="E122" t="s">
-        <v>579</v>
+        <v>650</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -7882,7 +7882,7 @@
         <v>582</v>
       </c>
       <c r="E123" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -7890,7 +7890,7 @@
         <v>368</v>
       </c>
       <c r="B124" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C124" t="s">
         <v>238</v>
@@ -7899,7 +7899,7 @@
         <v>583</v>
       </c>
       <c r="E124" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -7907,16 +7907,16 @@
         <v>369</v>
       </c>
       <c r="B125" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
       <c r="C125" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D125" t="s">
         <v>584</v>
       </c>
       <c r="E125" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -7941,16 +7941,16 @@
         <v>371</v>
       </c>
       <c r="B127" t="s">
-        <v>454</v>
+        <v>233</v>
       </c>
       <c r="C127" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D127" t="s">
         <v>586</v>
       </c>
       <c r="E127" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -7958,16 +7958,16 @@
         <v>372</v>
       </c>
       <c r="B128" t="s">
-        <v>233</v>
+        <v>460</v>
       </c>
       <c r="C128" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D128" t="s">
         <v>587</v>
       </c>
       <c r="E128" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -7975,7 +7975,7 @@
         <v>373</v>
       </c>
       <c r="B129" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="C129" t="s">
         <v>238</v>
@@ -7984,7 +7984,7 @@
         <v>588</v>
       </c>
       <c r="E129" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -7992,16 +7992,16 @@
         <v>374</v>
       </c>
       <c r="B130" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="C130" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D130" t="s">
         <v>589</v>
       </c>
       <c r="E130" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -8009,7 +8009,7 @@
         <v>375</v>
       </c>
       <c r="B131" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="C131" t="s">
         <v>238</v>
@@ -8018,7 +8018,7 @@
         <v>590</v>
       </c>
       <c r="E131" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -8035,7 +8035,7 @@
         <v>591</v>
       </c>
       <c r="E132" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -8060,16 +8060,16 @@
         <v>378</v>
       </c>
       <c r="B134" t="s">
-        <v>471</v>
+        <v>445</v>
       </c>
       <c r="C134" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D134" t="s">
         <v>593</v>
       </c>
       <c r="E134" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -8077,16 +8077,16 @@
         <v>379</v>
       </c>
       <c r="B135" t="s">
-        <v>444</v>
+        <v>471</v>
       </c>
       <c r="C135" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D135" t="s">
         <v>594</v>
       </c>
       <c r="E135" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -8103,7 +8103,7 @@
         <v>595</v>
       </c>
       <c r="E136" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -8145,16 +8145,16 @@
         <v>383</v>
       </c>
       <c r="B139" t="s">
-        <v>232</v>
+        <v>475</v>
       </c>
       <c r="C139" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D139" t="s">
         <v>598</v>
       </c>
       <c r="E139" t="s">
-        <v>653</v>
+        <v>601</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -8162,16 +8162,16 @@
         <v>384</v>
       </c>
       <c r="B140" t="s">
-        <v>475</v>
+        <v>232</v>
       </c>
       <c r="C140" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D140" t="s">
         <v>599</v>
       </c>
       <c r="E140" t="s">
-        <v>601</v>
+        <v>653</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -8205,7 +8205,7 @@
         <v>601</v>
       </c>
       <c r="E142" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -8222,7 +8222,7 @@
         <v>602</v>
       </c>
       <c r="E143" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -8230,16 +8230,16 @@
         <v>388</v>
       </c>
       <c r="B144" t="s">
-        <v>232</v>
+        <v>479</v>
       </c>
       <c r="C144" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D144" t="s">
         <v>603</v>
       </c>
       <c r="E144" t="s">
-        <v>654</v>
+        <v>604</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -8247,10 +8247,10 @@
         <v>389</v>
       </c>
       <c r="B145" t="s">
-        <v>479</v>
+        <v>445</v>
       </c>
       <c r="C145" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D145" t="s">
         <v>604</v>
@@ -8264,16 +8264,16 @@
         <v>390</v>
       </c>
       <c r="B146" t="s">
-        <v>444</v>
+        <v>232</v>
       </c>
       <c r="C146" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D146" t="s">
         <v>605</v>
       </c>
       <c r="E146" t="s">
-        <v>603</v>
+        <v>654</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -8290,7 +8290,7 @@
         <v>606</v>
       </c>
       <c r="E147" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -8307,7 +8307,7 @@
         <v>607</v>
       </c>
       <c r="E148" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -8315,7 +8315,7 @@
         <v>393</v>
       </c>
       <c r="B149" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C149" t="s">
         <v>238</v>
@@ -8324,7 +8324,7 @@
         <v>608</v>
       </c>
       <c r="E149" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -8332,16 +8332,16 @@
         <v>394</v>
       </c>
       <c r="B150" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C150" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D150" t="s">
         <v>609</v>
       </c>
       <c r="E150" t="s">
-        <v>610</v>
+        <v>655</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -8358,7 +8358,7 @@
         <v>610</v>
       </c>
       <c r="E151" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -8366,7 +8366,7 @@
         <v>396</v>
       </c>
       <c r="B152" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C152" t="s">
         <v>238</v>
@@ -8375,7 +8375,7 @@
         <v>611</v>
       </c>
       <c r="E152" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -8383,16 +8383,16 @@
         <v>397</v>
       </c>
       <c r="B153" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C153" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D153" t="s">
         <v>612</v>
       </c>
       <c r="E153" t="s">
-        <v>655</v>
+        <v>610</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -8400,16 +8400,16 @@
         <v>398</v>
       </c>
       <c r="B154" t="s">
-        <v>480</v>
+        <v>445</v>
       </c>
       <c r="C154" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D154" t="s">
         <v>613</v>
       </c>
       <c r="E154" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -8417,16 +8417,16 @@
         <v>399</v>
       </c>
       <c r="B155" t="s">
-        <v>444</v>
+        <v>478</v>
       </c>
       <c r="C155" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D155" t="s">
         <v>614</v>
       </c>
       <c r="E155" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -8451,7 +8451,7 @@
         <v>401</v>
       </c>
       <c r="B157" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="C157" t="s">
         <v>238</v>
@@ -8460,7 +8460,7 @@
         <v>616</v>
       </c>
       <c r="E157" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -8468,7 +8468,7 @@
         <v>402</v>
       </c>
       <c r="B158" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="C158" t="s">
         <v>238</v>
@@ -8477,7 +8477,7 @@
         <v>617</v>
       </c>
       <c r="E158" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -8485,7 +8485,7 @@
         <v>403</v>
       </c>
       <c r="B159" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C159" t="s">
         <v>238</v>
@@ -8494,7 +8494,7 @@
         <v>618</v>
       </c>
       <c r="E159" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -8502,16 +8502,16 @@
         <v>404</v>
       </c>
       <c r="B160" t="s">
-        <v>483</v>
+        <v>213</v>
       </c>
       <c r="C160" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D160" t="s">
         <v>619</v>
       </c>
       <c r="E160" t="s">
-        <v>620</v>
+        <v>657</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -8519,7 +8519,7 @@
         <v>405</v>
       </c>
       <c r="B161" t="s">
-        <v>469</v>
+        <v>233</v>
       </c>
       <c r="C161" t="s">
         <v>239</v>
@@ -8528,7 +8528,7 @@
         <v>620</v>
       </c>
       <c r="E161" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -8536,16 +8536,16 @@
         <v>406</v>
       </c>
       <c r="B162" t="s">
-        <v>213</v>
+        <v>484</v>
       </c>
       <c r="C162" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D162" t="s">
         <v>621</v>
       </c>
       <c r="E162" t="s">
-        <v>657</v>
+        <v>624</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -8553,7 +8553,7 @@
         <v>407</v>
       </c>
       <c r="B163" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C163" t="s">
         <v>238</v>
@@ -8562,7 +8562,7 @@
         <v>622</v>
       </c>
       <c r="E163" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -8570,16 +8570,16 @@
         <v>408</v>
       </c>
       <c r="B164" t="s">
-        <v>233</v>
+        <v>475</v>
       </c>
       <c r="C164" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D164" t="s">
         <v>623</v>
       </c>
       <c r="E164" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -8587,10 +8587,10 @@
         <v>409</v>
       </c>
       <c r="B165" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
       <c r="C165" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D165" t="s">
         <v>624</v>
@@ -8613,7 +8613,7 @@
         <v>625</v>
       </c>
       <c r="E166" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -8621,16 +8621,16 @@
         <v>411</v>
       </c>
       <c r="B167" t="s">
-        <v>213</v>
+        <v>479</v>
       </c>
       <c r="C167" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D167" t="s">
         <v>626</v>
       </c>
       <c r="E167" t="s">
-        <v>658</v>
+        <v>629</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -8638,7 +8638,7 @@
         <v>412</v>
       </c>
       <c r="B168" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="C168" t="s">
         <v>238</v>
@@ -8647,7 +8647,7 @@
         <v>627</v>
       </c>
       <c r="E168" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -8655,16 +8655,16 @@
         <v>413</v>
       </c>
       <c r="B169" t="s">
-        <v>444</v>
+        <v>213</v>
       </c>
       <c r="C169" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D169" t="s">
         <v>628</v>
       </c>
       <c r="E169" t="s">
-        <v>626</v>
+        <v>658</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -8672,10 +8672,10 @@
         <v>414</v>
       </c>
       <c r="B170" t="s">
-        <v>487</v>
+        <v>445</v>
       </c>
       <c r="C170" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D170" t="s">
         <v>629</v>
@@ -8689,7 +8689,7 @@
         <v>415</v>
       </c>
       <c r="B171" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C171" t="s">
         <v>238</v>
@@ -8698,7 +8698,7 @@
         <v>630</v>
       </c>
       <c r="E171" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>